<commit_message>
DOC: Update PRooFPS-dd v0.2.7.0 Calculations
</commit_message>
<xml_diff>
--- a/PGE/docpages/PRooFPS-dd-Packet-Rates.xlsx
+++ b/PGE/docpages/PRooFPS-dd-Packet-Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PGE\PGE\docpages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ADA250-A0D1-4D59-9961-D9039024238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CA120-188A-4964-9E4F-AAD31A7C858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
   <si>
     <t>v0.1.2</t>
   </si>
@@ -100,9 +100,6 @@
     <t>v0.1.0</t>
   </si>
   <si>
-    <t>Comment on Networking</t>
-  </si>
-  <si>
     <t>UserUpdate FromServer</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>1 packet i.e. PgePacket might contain 1 or more message. But until now it is always only exactly 1 message.</t>
   </si>
   <si>
-    <t>This is because we always calculate with PgePacket size that the engine is handing over to GNS layer. PgePacket = header + message.</t>
-  </si>
-  <si>
     <t>Only the frequently sent / received messages are listed, no connect / disconnect / config messages present in table.</t>
   </si>
   <si>
@@ -281,6 +275,36 @@
   </si>
   <si>
     <t>In Server Rx column, we see the received packet data rate from ALL players (1 out of 8 MsgUserCmdFromClient packets are injected by server to self (since those are from the server player itself).</t>
+  </si>
+  <si>
+    <t>This is because we always calculate with PgePacket size that the engine is handing over to GNS layer. PgePacket = header + message. PgePacket overhead is 15 Bytes.</t>
+  </si>
+  <si>
+    <t>Message sizes (without PgePacket overhead added) are also logged by the game after starting it up and entered to main menu.</t>
+  </si>
+  <si>
+    <t>The aim is to keep the packet rate much far away from the v0.1.0 levels because with that version serious packet congestion occurred!</t>
+  </si>
+  <si>
+    <t>The aim is to keep the packet data rate much far away from the v0.1.0 levels because with that version serious packet congestion occurred!</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Armor added to UserUpdateFromServer, Weapon states added to WpnUpdateFromServer.</t>
+  </si>
+  <si>
+    <t>More bullet properties replicated.</t>
+  </si>
+  <si>
+    <t>Added fSomersaultAngleZ.</t>
+  </si>
+  <si>
+    <t>Added player invulnerability state, and weapon states added to CurrentWpnUpdateFromServer.</t>
+  </si>
+  <si>
+    <t>Added nMapItemType and nAmmoIncrease to WpnUpdateFromServer.</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1130,8 +1154,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1147,19 +1169,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1178,6 +1187,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,6 +1226,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1241,9 +1310,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,39 +1322,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1301,25 +1334,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1663,13 +1699,13 @@
       <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
@@ -1684,7 +1720,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1694,58 +1730,61 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="69" t="s">
+      <c r="A10" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
+    </row>
+    <row r="11" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="71"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
-    </row>
-    <row r="11" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="61" t="s">
+      <c r="E11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="G11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>23</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>24</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1758,29 +1797,29 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="56">
+      <c r="C12" s="111">
         <v>268</v>
       </c>
-      <c r="D12" s="57">
+      <c r="D12" s="112">
         <v>268</v>
       </c>
-      <c r="E12" s="58">
+      <c r="E12" s="113">
         <v>268</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="113">
         <v>268</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="113">
         <v>268</v>
       </c>
-      <c r="H12" s="59">
+      <c r="H12" s="114">
         <v>268</v>
       </c>
       <c r="I12" s="5"/>
@@ -1794,25 +1833,25 @@
       <c r="A13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="52">
+      <c r="B13" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="42">
         <v>268</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="59">
         <v>268</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="10">
         <v>268</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="10">
         <v>268</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="10">
         <v>268</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="115">
         <v>268</v>
       </c>
       <c r="I13" s="5"/>
@@ -1826,25 +1865,25 @@
       <c r="A14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="52">
+      <c r="B14" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="42">
         <v>268</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D14" s="59">
         <v>268</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="10">
         <v>268</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="10">
         <v>268</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="10">
         <v>268</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="115">
         <v>268</v>
       </c>
       <c r="I14" s="5"/>
@@ -1858,25 +1897,25 @@
       <c r="A15" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="52">
+      <c r="B15" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="42">
         <v>268</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="59">
         <v>268</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="10">
         <v>268</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="10">
         <v>268</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="10">
         <v>268</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="115">
         <v>268</v>
       </c>
       <c r="I15" s="5"/>
@@ -1890,25 +1929,25 @@
       <c r="A16" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="42">
         <v>31</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="59">
         <v>55</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="10">
         <v>23</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="10">
         <v>91</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="10">
         <v>79</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="115">
         <v>71</v>
       </c>
       <c r="I16" s="5"/>
@@ -1922,25 +1961,25 @@
       <c r="A17" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="42">
         <v>31</v>
       </c>
-      <c r="C17" s="52">
-        <v>31</v>
-      </c>
-      <c r="D17" s="50">
+      <c r="D17" s="59">
         <v>55</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="10">
         <v>23</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="10">
         <v>91</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="10">
         <v>79</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="115">
         <v>71</v>
       </c>
       <c r="I17" s="5"/>
@@ -1954,25 +1993,25 @@
       <c r="A18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="42">
         <v>31</v>
       </c>
-      <c r="C18" s="52">
-        <v>31</v>
-      </c>
-      <c r="D18" s="50">
+      <c r="D18" s="59">
         <v>55</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="10">
         <v>23</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="10">
         <v>91</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="10">
         <v>79</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="115">
         <v>71</v>
       </c>
       <c r="I18" s="5"/>
@@ -1986,25 +2025,25 @@
       <c r="A19" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="42">
         <v>31</v>
       </c>
-      <c r="C19" s="52">
-        <v>31</v>
-      </c>
-      <c r="D19" s="50">
+      <c r="D19" s="59">
         <v>55</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="10">
         <v>23</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="10">
         <v>91</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="10">
         <v>79</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="115">
         <v>83</v>
       </c>
       <c r="I19" s="5"/>
@@ -2018,25 +2057,25 @@
       <c r="A20" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="42">
         <v>31</v>
       </c>
-      <c r="C20" s="52">
-        <v>31</v>
-      </c>
-      <c r="D20" s="50">
+      <c r="D20" s="59">
         <v>55</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="10">
         <v>23</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="10">
         <v>91</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="10">
         <v>79</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="115">
         <v>83</v>
       </c>
       <c r="I20" s="5"/>
@@ -2050,25 +2089,25 @@
       <c r="A21" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="109" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="42">
         <v>31</v>
       </c>
-      <c r="C21" s="52">
-        <v>31</v>
-      </c>
-      <c r="D21" s="50">
+      <c r="D21" s="59">
         <v>63</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="10">
         <v>23</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="10">
         <v>91</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="10">
         <v>79</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="115">
         <v>83</v>
       </c>
       <c r="I21" s="5"/>
@@ -2078,29 +2117,29 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="109" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="42">
         <v>31</v>
       </c>
-      <c r="C22" s="52">
-        <v>31</v>
-      </c>
-      <c r="D22" s="50">
+      <c r="D22" s="59">
         <v>67</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="10">
         <v>23</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="10">
         <v>91</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="10">
         <v>83</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="115">
         <v>83</v>
       </c>
       <c r="I22" s="5"/>
@@ -2114,25 +2153,25 @@
       <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="42">
         <v>31</v>
       </c>
-      <c r="C23" s="52">
-        <v>31</v>
-      </c>
-      <c r="D23" s="50">
+      <c r="D23" s="59">
         <v>67</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="10">
         <v>23</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="10">
         <v>91</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="10">
         <v>83</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="115">
         <v>83</v>
       </c>
       <c r="I23" s="5"/>
@@ -2146,25 +2185,25 @@
       <c r="A24" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="42">
         <v>31</v>
       </c>
-      <c r="C24" s="52">
-        <v>31</v>
-      </c>
-      <c r="D24" s="50">
+      <c r="D24" s="59">
         <v>67</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="10">
         <v>23</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="10">
         <v>91</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="10">
         <v>83</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="115">
         <v>83</v>
       </c>
       <c r="I24" s="5"/>
@@ -2174,29 +2213,29 @@
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="42">
         <v>31</v>
       </c>
-      <c r="C25" s="52">
-        <v>31</v>
-      </c>
-      <c r="D25" s="50">
+      <c r="D25" s="59">
         <v>67</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="10">
         <v>23</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="10">
         <v>99</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="10">
         <v>83</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="115">
         <v>83</v>
       </c>
       <c r="I25" s="5"/>
@@ -2206,21 +2245,37 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="109" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="42">
+        <f>16+15</f>
         <v>31</v>
       </c>
-      <c r="C26" s="52">
-        <v>31</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="32"/>
+      <c r="D26" s="59">
+        <f>56+15</f>
+        <v>71</v>
+      </c>
+      <c r="E26" s="10">
+        <f>8+15</f>
+        <v>23</v>
+      </c>
+      <c r="F26" s="10">
+        <f>88+15</f>
+        <v>103</v>
+      </c>
+      <c r="G26" s="10">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
+      <c r="H26" s="115">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -2230,9 +2285,9 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="50"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -2246,9 +2301,9 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="50"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -2262,9 +2317,9 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="50"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -2278,9 +2333,9 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="50"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -2294,9 +2349,9 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="50"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -2310,9 +2365,9 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="50"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
@@ -2326,9 +2381,9 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="50"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
@@ -2342,9 +2397,9 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="45"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="51"/>
+      <c r="B34" s="110"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
       <c r="G34" s="46"/>
@@ -2474,16 +2529,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C73525B-4602-4ED0-8F77-5C69A22A2F34}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="D30" sqref="D30"/>
+      <selection pane="topRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
@@ -2501,32 +2556,32 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -2534,86 +2589,86 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <f>C9+1</f>
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <f>C10*6</f>
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14">
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -2621,141 +2676,144 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="76" t="s">
+      <c r="A27" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="96"/>
+      <c r="E27" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="96"/>
+    </row>
+    <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="87"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="O27" s="82"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="83"/>
-    </row>
-    <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="74"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="107" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="100" t="s">
+      <c r="F28" s="77"/>
+      <c r="G28" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" s="91"/>
-      <c r="L28" s="101" t="s">
+      <c r="H28" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="M28" s="102"/>
-      <c r="N28" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="O28" s="86"/>
-      <c r="P28" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q28" s="80"/>
+      <c r="I28" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="103"/>
+      <c r="L28" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" s="79"/>
+      <c r="N28" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="O28" s="99"/>
+      <c r="P28" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q28" s="93"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="108"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="88"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="88"/>
+        <v>64</v>
+      </c>
+      <c r="G29" s="100"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="100"/>
       <c r="J29" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K29" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P29" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q29" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2763,21 +2821,21 @@
         <v>19</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="41">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="D30" s="109">
+      <c r="D30" s="60">
         <f>1-(C30/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="96">
+      <c r="E30" s="85">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="F30" s="92"/>
+      <c r="F30" s="82"/>
       <c r="G30" s="7">
         <f>$C$10*$C$13</f>
         <v>480</v>
@@ -2790,13 +2848,13 @@
         <f>$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J30" s="92">
+      <c r="J30" s="82">
         <f>$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K30" s="93"/>
+      <c r="K30" s="83"/>
       <c r="L30" s="23">
-        <f t="shared" ref="L30:L43" si="0">E30+G30+H30+I30+J30</f>
+        <f t="shared" ref="L30:L44" si="0">E30+G30+H30+I30+J30</f>
         <v>4327</v>
       </c>
       <c r="M30" s="8">
@@ -2811,11 +2869,11 @@
         <f>7*M30</f>
         <v>30289</v>
       </c>
-      <c r="P30" s="63">
+      <c r="P30" s="56">
         <f>1-(N30/$N$30)</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="64">
+      <c r="Q30" s="57">
         <f>1-(O30/$O$30)</f>
         <v>0</v>
       </c>
@@ -2831,21 +2889,21 @@
         <v>18</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" s="42">
         <f t="shared" ref="C31:G33" si="1">$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="D31" s="110">
+      <c r="D31" s="61">
         <f t="shared" ref="D31:D51" si="2">1-(C31/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="97">
+      <c r="E31" s="72">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F31" s="94"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2858,11 +2916,11 @@
         <f t="shared" ref="I31:I33" si="4">$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J31" s="94">
+      <c r="J31" s="73">
         <f t="shared" ref="J31:J32" si="5">$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K31" s="95"/>
+      <c r="K31" s="84"/>
       <c r="L31" s="24">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -2872,18 +2930,18 @@
         <v>4327</v>
       </c>
       <c r="N31" s="24">
-        <f t="shared" ref="N31:N43" si="6">7*L31</f>
+        <f t="shared" ref="N31:N44" si="6">7*L31</f>
         <v>30289</v>
       </c>
       <c r="O31" s="11">
-        <f t="shared" ref="O31:O43" si="7">7*M31</f>
+        <f t="shared" ref="O31:O44" si="7">7*M31</f>
         <v>30289</v>
       </c>
-      <c r="P31" s="63">
+      <c r="P31" s="56">
         <f t="shared" ref="P31:P51" si="8">1-(N31/$N$30)</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="64">
+      <c r="Q31" s="57">
         <f t="shared" ref="Q31:Q51" si="9">1-(O31/$O$30)</f>
         <v>0</v>
       </c>
@@ -2899,21 +2957,21 @@
         <v>0</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="42">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D32" s="110">
+      <c r="D32" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E32" s="97">
+      <c r="E32" s="72">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F32" s="94"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2926,11 +2984,11 @@
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J32" s="94">
+      <c r="J32" s="73">
         <f t="shared" si="5"/>
         <v>2880</v>
       </c>
-      <c r="K32" s="95"/>
+      <c r="K32" s="84"/>
       <c r="L32" s="24">
         <f t="shared" si="0"/>
         <v>4327</v>
@@ -2947,11 +3005,11 @@
         <f t="shared" si="7"/>
         <v>30289</v>
       </c>
-      <c r="P32" s="63">
+      <c r="P32" s="56">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="64">
+      <c r="Q32" s="57">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2967,21 +3025,21 @@
         <v>1</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="42">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D33" s="110">
+      <c r="D33" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="97">
+      <c r="E33" s="72">
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F33" s="94"/>
+      <c r="F33" s="73"/>
       <c r="G33" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3018,11 +3076,11 @@
         <f t="shared" si="7"/>
         <v>12089</v>
       </c>
-      <c r="P33" s="63">
+      <c r="P33" s="56">
         <f t="shared" si="8"/>
         <v>0.60087820660966029</v>
       </c>
-      <c r="Q33" s="64">
+      <c r="Q33" s="57">
         <f t="shared" si="9"/>
         <v>0.60087820660966029</v>
       </c>
@@ -3038,21 +3096,21 @@
         <v>2</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="42">
         <f>16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D34" s="110">
+      <c r="D34" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
-      <c r="E34" s="97">
+      <c r="E34" s="72">
         <f t="shared" ref="E34" si="10">$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F34" s="94"/>
+      <c r="F34" s="73"/>
       <c r="G34" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3089,11 +3147,11 @@
         <f t="shared" si="7"/>
         <v>3647</v>
       </c>
-      <c r="P34" s="63">
+      <c r="P34" s="56">
         <f t="shared" si="8"/>
         <v>0.87959325167552582</v>
       </c>
-      <c r="Q34" s="64">
+      <c r="Q34" s="57">
         <f t="shared" si="9"/>
         <v>0.87959325167552582</v>
       </c>
@@ -3109,13 +3167,13 @@
         <v>3</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="42">
-        <f t="shared" ref="C35:C43" si="11">16*$C$10</f>
+        <f t="shared" ref="C35:C44" si="11">16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D35" s="110">
+      <c r="D35" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3124,7 +3182,7 @@
         <v>160</v>
       </c>
       <c r="F35" s="10">
-        <f t="shared" ref="F35:F43" si="12">$C$10*$C$16</f>
+        <f t="shared" ref="F35:F44" si="12">$C$10*$C$16</f>
         <v>480</v>
       </c>
       <c r="G35" s="10">
@@ -3140,11 +3198,11 @@
         <v>14</v>
       </c>
       <c r="J35" s="10">
-        <f t="shared" ref="J35:J43" si="14">$C$10*$C$15</f>
+        <f t="shared" ref="J35:J44" si="14">$C$10*$C$15</f>
         <v>160</v>
       </c>
       <c r="K35" s="22">
-        <f t="shared" ref="K35:K43" si="15">$C$10*$C$14</f>
+        <f t="shared" ref="K35:K44" si="15">$C$10*$C$14</f>
         <v>480</v>
       </c>
       <c r="L35" s="24">
@@ -3152,7 +3210,7 @@
         <v>881</v>
       </c>
       <c r="M35" s="11">
-        <f t="shared" ref="M35:M43" si="16">F35+G35+H35+I35+K35</f>
+        <f t="shared" ref="M35:M44" si="16">F35+G35+H35+I35+K35</f>
         <v>1521</v>
       </c>
       <c r="N35" s="24">
@@ -3163,11 +3221,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P35" s="63">
+      <c r="P35" s="56">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q35" s="64">
+      <c r="Q35" s="57">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3183,18 +3241,18 @@
         <v>4</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D36" s="110">
+      <c r="D36" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
       <c r="E36" s="9">
-        <f t="shared" ref="E36:E43" si="17">$C$10*$C$17</f>
+        <f t="shared" ref="E36:E44" si="17">$C$10*$C$17</f>
         <v>160</v>
       </c>
       <c r="F36" s="10">
@@ -3202,11 +3260,11 @@
         <v>480</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" ref="G36:G43" si="18">$C$10*$C$14</f>
+        <f t="shared" ref="G36:G44" si="18">$C$10*$C$14</f>
         <v>480</v>
       </c>
       <c r="H36" s="22">
-        <f t="shared" ref="H36:H43" si="19">7 + 1*$C$13</f>
+        <f t="shared" ref="H36:H44" si="19">7 + 1*$C$13</f>
         <v>67</v>
       </c>
       <c r="I36" s="10">
@@ -3237,11 +3295,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P36" s="63">
+      <c r="P36" s="56">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q36" s="64">
+      <c r="Q36" s="57">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3257,13 +3315,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C37" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D37" s="110">
+      <c r="D37" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3311,11 +3369,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P37" s="63">
+      <c r="P37" s="56">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q37" s="64">
+      <c r="Q37" s="57">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3331,13 +3389,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C38" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D38" s="110">
+      <c r="D38" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3385,11 +3443,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P38" s="63">
+      <c r="P38" s="56">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q38" s="64">
+      <c r="Q38" s="57">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3405,13 +3463,13 @@
         <v>7</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D39" s="110">
+      <c r="D39" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3459,11 +3517,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P39" s="63">
+      <c r="P39" s="56">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q39" s="64">
+      <c r="Q39" s="57">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3479,13 +3537,13 @@
         <v>8</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C40" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D40" s="110">
+      <c r="D40" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3533,11 +3591,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P40" s="63">
+      <c r="P40" s="56">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q40" s="64">
+      <c r="Q40" s="57">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3553,13 +3611,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C41" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D41" s="110">
+      <c r="D41" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3580,7 +3638,7 @@
         <v>67</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" ref="I41:I43" si="20">$C$9*2 + $C$9*2</f>
+        <f t="shared" ref="I41:I44" si="20">$C$9*2 + $C$9*2</f>
         <v>28</v>
       </c>
       <c r="J41" s="10">
@@ -3607,11 +3665,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P41" s="63">
+      <c r="P41" s="56">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q41" s="64">
+      <c r="Q41" s="57">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3627,13 +3685,13 @@
         <v>10</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D42" s="110">
+      <c r="D42" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3681,11 +3739,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P42" s="63">
+      <c r="P42" s="56">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q42" s="64">
+      <c r="Q42" s="57">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3701,13 +3759,13 @@
         <v>11</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" s="42">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D43" s="110">
+      <c r="D43" s="61">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3755,11 +3813,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P43" s="63">
+      <c r="P43" s="56">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q43" s="64">
+      <c r="Q43" s="57">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3775,31 +3833,67 @@
         <v>12</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="110">
+        <v>29</v>
+      </c>
+      <c r="C44" s="42">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+      <c r="D44" s="61">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="63">
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="E44" s="9">
+        <f t="shared" si="17"/>
+        <v>160</v>
+      </c>
+      <c r="F44" s="10">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="G44" s="10">
+        <f t="shared" si="18"/>
+        <v>480</v>
+      </c>
+      <c r="H44" s="22">
+        <f t="shared" si="19"/>
+        <v>67</v>
+      </c>
+      <c r="I44" s="10">
+        <f t="shared" si="20"/>
+        <v>28</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="14"/>
+        <v>160</v>
+      </c>
+      <c r="K44" s="22">
+        <f t="shared" si="15"/>
+        <v>480</v>
+      </c>
+      <c r="L44" s="24">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
+      <c r="M44" s="11">
+        <f t="shared" si="16"/>
+        <v>1535</v>
+      </c>
+      <c r="N44" s="24">
+        <f t="shared" si="6"/>
+        <v>6265</v>
+      </c>
+      <c r="O44" s="11">
+        <f t="shared" si="7"/>
+        <v>10745</v>
+      </c>
+      <c r="P44" s="56">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q44" s="64">
+        <v>0.79315923272475153</v>
+      </c>
+      <c r="Q44" s="57">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.64525075109775831</v>
       </c>
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
@@ -3812,10 +3906,7 @@
       <c r="A45" s="34"/>
       <c r="B45" s="35"/>
       <c r="C45" s="43"/>
-      <c r="D45" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D45" s="61"/>
       <c r="E45" s="12"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
@@ -3827,14 +3918,8 @@
       <c r="M45" s="14"/>
       <c r="N45" s="25"/>
       <c r="O45" s="26"/>
-      <c r="P45" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q45" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="57"/>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
@@ -3846,10 +3931,7 @@
       <c r="A46" s="34"/>
       <c r="B46" s="35"/>
       <c r="C46" s="43"/>
-      <c r="D46" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D46" s="61"/>
       <c r="E46" s="12"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -3861,14 +3943,8 @@
       <c r="M46" s="14"/>
       <c r="N46" s="25"/>
       <c r="O46" s="26"/>
-      <c r="P46" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q46" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="57"/>
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
@@ -3880,10 +3956,7 @@
       <c r="A47" s="34"/>
       <c r="B47" s="35"/>
       <c r="C47" s="43"/>
-      <c r="D47" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D47" s="61"/>
       <c r="E47" s="12"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -3895,14 +3968,8 @@
       <c r="M47" s="14"/>
       <c r="N47" s="25"/>
       <c r="O47" s="26"/>
-      <c r="P47" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q47" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="57"/>
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
@@ -3914,10 +3981,7 @@
       <c r="A48" s="34"/>
       <c r="B48" s="35"/>
       <c r="C48" s="43"/>
-      <c r="D48" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D48" s="61"/>
       <c r="E48" s="12"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -3929,14 +3993,8 @@
       <c r="M48" s="14"/>
       <c r="N48" s="25"/>
       <c r="O48" s="26"/>
-      <c r="P48" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q48" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P48" s="56"/>
+      <c r="Q48" s="57"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
       <c r="T48" s="4"/>
@@ -3948,10 +4006,7 @@
       <c r="A49" s="34"/>
       <c r="B49" s="35"/>
       <c r="C49" s="43"/>
-      <c r="D49" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D49" s="61"/>
       <c r="E49" s="12"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
@@ -3963,14 +4018,8 @@
       <c r="M49" s="14"/>
       <c r="N49" s="25"/>
       <c r="O49" s="26"/>
-      <c r="P49" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q49" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="57"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
@@ -3982,10 +4031,7 @@
       <c r="A50" s="34"/>
       <c r="B50" s="35"/>
       <c r="C50" s="43"/>
-      <c r="D50" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D50" s="61"/>
       <c r="E50" s="12"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -3997,14 +4043,8 @@
       <c r="M50" s="14"/>
       <c r="N50" s="25"/>
       <c r="O50" s="26"/>
-      <c r="P50" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q50" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P50" s="56"/>
+      <c r="Q50" s="57"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
@@ -4016,10 +4056,7 @@
       <c r="A51" s="36"/>
       <c r="B51" s="37"/>
       <c r="C51" s="44"/>
-      <c r="D51" s="110">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+      <c r="D51" s="61"/>
       <c r="E51" s="15"/>
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
@@ -4031,14 +4068,8 @@
       <c r="M51" s="17"/>
       <c r="N51" s="27"/>
       <c r="O51" s="28"/>
-      <c r="P51" s="63">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Q51" s="64">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="P51" s="56"/>
+      <c r="Q51" s="57"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
@@ -4049,7 +4080,7 @@
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="111"/>
+      <c r="D52" s="62"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -4061,8 +4092,8 @@
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
-      <c r="P52" s="65"/>
-      <c r="Q52" s="65"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="58"/>
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
@@ -4119,16 +4150,27 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C28:C29"/>
@@ -4141,23 +4183,12 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D51">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4165,11 +4196,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30:F51">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="D30:D51">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:F51">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4178,10 +4221,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:G51">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4190,10 +4233,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30:H51">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4202,10 +4245,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I51">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4214,10 +4257,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:K51">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4226,10 +4269,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:M51">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -4237,23 +4280,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30:P51">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P30:P51">
+  <conditionalFormatting sqref="P30:Q44">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -4261,27 +4292,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q30:Q51">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D51">
+  <conditionalFormatting sqref="N30:O44">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="30"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -4293,15 +4312,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A631036-56BD-4CE5-917C-895C0C771D72}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I35" sqref="I35"/>
+      <selection pane="topRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
@@ -4320,170 +4339,175 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="76" t="s">
+      <c r="A15" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="96"/>
+      <c r="E15" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="96"/>
+    </row>
+    <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="87"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="83"/>
-      <c r="E15" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="83"/>
-    </row>
-    <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="107" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="100" t="s">
+      <c r="F16" s="77"/>
+      <c r="G16" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="91"/>
-      <c r="L16" s="101" t="s">
+      <c r="H16" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="102"/>
-      <c r="N16" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="O16" s="86"/>
-      <c r="P16" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" s="80"/>
+      <c r="I16" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="103"/>
+      <c r="L16" s="78" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="79"/>
+      <c r="N16" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="99"/>
+      <c r="P16" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q16" s="93"/>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="108"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="88"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="88"/>
+        <v>64</v>
+      </c>
+      <c r="G17" s="100"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="100"/>
       <c r="J17" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L17" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="30"/>
+      <c r="B18" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="C18" s="41">
         <f>'Packet Rates'!C30*'Packet Sizes'!C12</f>
         <v>128640</v>
       </c>
-      <c r="D18" s="112">
+      <c r="D18" s="63">
         <f>1-(C18/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="103">
+      <c r="E18" s="104">
         <f>'Packet Rates'!E30*'Packet Sizes'!D12</f>
         <v>128640</v>
       </c>
-      <c r="F18" s="104"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="7">
         <f>'Packet Rates'!G30*'Packet Sizes'!E12</f>
         <v>128640</v>
@@ -4496,11 +4520,11 @@
         <f>'Packet Rates'!I30*'Packet Sizes'!G12</f>
         <v>112560</v>
       </c>
-      <c r="J18" s="92">
+      <c r="J18" s="82">
         <f>'Packet Rates'!J30*'Packet Sizes'!H12</f>
         <v>771840</v>
       </c>
-      <c r="K18" s="93"/>
+      <c r="K18" s="83"/>
       <c r="L18" s="23">
         <f>E18+G18+H18+I18+J18</f>
         <v>1159636</v>
@@ -4517,11 +4541,11 @@
         <f>M18*7</f>
         <v>8117452</v>
       </c>
-      <c r="P18" s="63">
+      <c r="P18" s="56">
         <f>1-(N18/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="64">
+      <c r="Q18" s="57">
         <f>1-(O18/$O$18)</f>
         <v>0</v>
       </c>
@@ -4530,20 +4554,22 @@
       <c r="A19" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C19" s="42">
         <f>'Packet Rates'!C31*'Packet Sizes'!C13</f>
         <v>128640</v>
       </c>
-      <c r="D19" s="113">
+      <c r="D19" s="64">
         <f t="shared" ref="D19:D39" si="0">1-(C19/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="105">
+      <c r="E19" s="106">
         <f>'Packet Rates'!E31*'Packet Sizes'!D13</f>
         <v>128640</v>
       </c>
-      <c r="F19" s="106"/>
+      <c r="F19" s="107"/>
       <c r="G19" s="10">
         <f>'Packet Rates'!G31*'Packet Sizes'!E13</f>
         <v>128640</v>
@@ -4556,13 +4582,13 @@
         <f>'Packet Rates'!I31*'Packet Sizes'!G13</f>
         <v>112560</v>
       </c>
-      <c r="J19" s="94">
+      <c r="J19" s="73">
         <f>'Packet Rates'!J31*'Packet Sizes'!H13</f>
         <v>771840</v>
       </c>
-      <c r="K19" s="95"/>
+      <c r="K19" s="84"/>
       <c r="L19" s="24">
-        <f t="shared" ref="L19:L31" si="1">E19+G19+H19+I19+J19</f>
+        <f t="shared" ref="L19:L32" si="1">E19+G19+H19+I19+J19</f>
         <v>1159636</v>
       </c>
       <c r="M19" s="11">
@@ -4570,18 +4596,18 @@
         <v>1159636</v>
       </c>
       <c r="N19" s="24">
-        <f t="shared" ref="N19:N31" si="3">L19*7</f>
+        <f t="shared" ref="N19:N32" si="3">L19*7</f>
         <v>8117452</v>
       </c>
       <c r="O19" s="11">
-        <f t="shared" ref="O19:O31" si="4">M19*7</f>
+        <f t="shared" ref="O19:O32" si="4">M19*7</f>
         <v>8117452</v>
       </c>
-      <c r="P19" s="63">
+      <c r="P19" s="56">
         <f t="shared" ref="P19:P39" si="5">1-(N19/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="64">
+      <c r="Q19" s="57">
         <f t="shared" ref="Q19:Q39" si="6">1-(O19/$O$18)</f>
         <v>0</v>
       </c>
@@ -4590,20 +4616,22 @@
       <c r="A20" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C20" s="42">
         <f>'Packet Rates'!C32*'Packet Sizes'!C14</f>
         <v>128640</v>
       </c>
-      <c r="D20" s="113">
+      <c r="D20" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="105">
+      <c r="E20" s="106">
         <f>'Packet Rates'!E32*'Packet Sizes'!D14</f>
         <v>128640</v>
       </c>
-      <c r="F20" s="106"/>
+      <c r="F20" s="107"/>
       <c r="G20" s="10">
         <f>'Packet Rates'!G32*'Packet Sizes'!E14</f>
         <v>128640</v>
@@ -4616,11 +4644,11 @@
         <f>'Packet Rates'!I32*'Packet Sizes'!G14</f>
         <v>112560</v>
       </c>
-      <c r="J20" s="94">
+      <c r="J20" s="73">
         <f>'Packet Rates'!J32*'Packet Sizes'!H14</f>
         <v>771840</v>
       </c>
-      <c r="K20" s="95"/>
+      <c r="K20" s="84"/>
       <c r="L20" s="24">
         <f t="shared" si="1"/>
         <v>1159636</v>
@@ -4637,11 +4665,11 @@
         <f t="shared" si="4"/>
         <v>8117452</v>
       </c>
-      <c r="P20" s="63">
+      <c r="P20" s="56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="64">
+      <c r="Q20" s="57">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4650,20 +4678,22 @@
       <c r="A21" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="33"/>
+      <c r="B21" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="C21" s="42">
         <f>'Packet Rates'!C33*'Packet Sizes'!C15</f>
         <v>128640</v>
       </c>
-      <c r="D21" s="113">
+      <c r="D21" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="97">
+      <c r="E21" s="72">
         <f>'Packet Rates'!E33*'Packet Sizes'!D15</f>
         <v>42880</v>
       </c>
-      <c r="F21" s="94"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="10">
         <f>'Packet Rates'!G33*'Packet Sizes'!E15</f>
         <v>42880</v>
@@ -4700,11 +4730,11 @@
         <f t="shared" si="4"/>
         <v>3239852</v>
       </c>
-      <c r="P21" s="63">
+      <c r="P21" s="56">
         <f t="shared" si="5"/>
         <v>0.60087820660966029</v>
       </c>
-      <c r="Q21" s="64">
+      <c r="Q21" s="57">
         <f t="shared" si="6"/>
         <v>0.60087820660966029</v>
       </c>
@@ -4713,20 +4743,22 @@
       <c r="A22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="C22" s="42">
         <f>'Packet Rates'!C34*'Packet Sizes'!C16</f>
         <v>3968</v>
       </c>
-      <c r="D22" s="113">
+      <c r="D22" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="72">
         <f>'Packet Rates'!E34*'Packet Sizes'!D16</f>
         <v>8800</v>
       </c>
-      <c r="F22" s="94"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="10">
         <f>'Packet Rates'!G34*'Packet Sizes'!E16</f>
         <v>3680</v>
@@ -4763,11 +4795,11 @@
         <f t="shared" si="4"/>
         <v>191821</v>
       </c>
-      <c r="P22" s="63">
+      <c r="P22" s="56">
         <f t="shared" si="5"/>
         <v>0.97636930899006236</v>
       </c>
-      <c r="Q22" s="64">
+      <c r="Q22" s="57">
         <f t="shared" si="6"/>
         <v>0.97636930899006236</v>
       </c>
@@ -4776,12 +4808,14 @@
       <c r="A23" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="33" t="s">
+        <v>29</v>
+      </c>
       <c r="C23" s="42">
         <f>'Packet Rates'!C35*'Packet Sizes'!C17</f>
         <v>3968</v>
       </c>
-      <c r="D23" s="113">
+      <c r="D23" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4829,11 +4863,11 @@
         <f t="shared" si="4"/>
         <v>551061</v>
       </c>
-      <c r="P23" s="63">
+      <c r="P23" s="56">
         <f t="shared" si="5"/>
         <v>0.96688357381109247</v>
       </c>
-      <c r="Q23" s="64">
+      <c r="Q23" s="57">
         <f t="shared" si="6"/>
         <v>0.93211404268235898</v>
       </c>
@@ -4842,12 +4876,14 @@
       <c r="A24" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="32"/>
+      <c r="B24" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C24" s="42">
         <f>'Packet Rates'!C36*'Packet Sizes'!C18</f>
         <v>3968</v>
       </c>
-      <c r="D24" s="113">
+      <c r="D24" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4884,7 +4920,7 @@
         <v>38403</v>
       </c>
       <c r="M24" s="11">
-        <f t="shared" ref="M24:M31" si="7">F24+G24+H24+I24+K24</f>
+        <f t="shared" ref="M24:M32" si="7">F24+G24+H24+I24+K24</f>
         <v>78723</v>
       </c>
       <c r="N24" s="24">
@@ -4895,11 +4931,11 @@
         <f t="shared" si="4"/>
         <v>551061</v>
       </c>
-      <c r="P24" s="63">
+      <c r="P24" s="56">
         <f t="shared" si="5"/>
         <v>0.96688357381109247</v>
       </c>
-      <c r="Q24" s="64">
+      <c r="Q24" s="57">
         <f t="shared" si="6"/>
         <v>0.93211404268235898</v>
       </c>
@@ -4908,12 +4944,14 @@
       <c r="A25" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="32"/>
+      <c r="B25" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C25" s="42">
         <f>'Packet Rates'!C37*'Packet Sizes'!C19</f>
         <v>3968</v>
       </c>
-      <c r="D25" s="113">
+      <c r="D25" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4961,11 +4999,11 @@
         <f t="shared" si="4"/>
         <v>591381</v>
       </c>
-      <c r="P25" s="63">
+      <c r="P25" s="56">
         <f t="shared" si="5"/>
         <v>0.96522788185258135</v>
       </c>
-      <c r="Q25" s="64">
+      <c r="Q25" s="57">
         <f t="shared" si="6"/>
         <v>0.92714696680682562</v>
       </c>
@@ -4974,12 +5012,14 @@
       <c r="A26" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C26" s="42">
         <f>'Packet Rates'!C38*'Packet Sizes'!C20</f>
         <v>3968</v>
       </c>
-      <c r="D26" s="113">
+      <c r="D26" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5027,11 +5067,11 @@
         <f t="shared" si="4"/>
         <v>591381</v>
       </c>
-      <c r="P26" s="63">
+      <c r="P26" s="56">
         <f t="shared" si="5"/>
         <v>0.96522788185258135</v>
       </c>
-      <c r="Q26" s="64">
+      <c r="Q26" s="57">
         <f t="shared" si="6"/>
         <v>0.92714696680682562</v>
       </c>
@@ -5040,12 +5080,14 @@
       <c r="A27" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C27" s="42">
         <f>'Packet Rates'!C39*'Packet Sizes'!C21</f>
         <v>3968</v>
       </c>
-      <c r="D27" s="113">
+      <c r="D27" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5093,11 +5135,11 @@
         <f t="shared" si="4"/>
         <v>618261</v>
       </c>
-      <c r="P27" s="63">
+      <c r="P27" s="56">
         <f t="shared" si="5"/>
         <v>0.9641240872135739</v>
       </c>
-      <c r="Q27" s="64">
+      <c r="Q27" s="57">
         <f t="shared" si="6"/>
         <v>0.92383558288980339</v>
       </c>
@@ -5106,12 +5148,14 @@
       <c r="A28" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="32"/>
+      <c r="B28" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C28" s="42">
         <f>'Packet Rates'!C40*'Packet Sizes'!C22</f>
         <v>3968</v>
       </c>
-      <c r="D28" s="113">
+      <c r="D28" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5159,11 +5203,11 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P28" s="63">
+      <c r="P28" s="56">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q28" s="64">
+      <c r="Q28" s="57">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
@@ -5172,12 +5216,14 @@
       <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="32"/>
+      <c r="B29" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C29" s="42">
         <f>'Packet Rates'!C41*'Packet Sizes'!C23</f>
         <v>3968</v>
       </c>
-      <c r="D29" s="113">
+      <c r="D29" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5225,11 +5271,11 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P29" s="63">
+      <c r="P29" s="56">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q29" s="64">
+      <c r="Q29" s="57">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
@@ -5238,12 +5284,14 @@
       <c r="A30" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C30" s="42">
         <f>'Packet Rates'!C42*'Packet Sizes'!C24</f>
         <v>3968</v>
       </c>
-      <c r="D30" s="113">
+      <c r="D30" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5291,11 +5339,11 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P30" s="63">
+      <c r="P30" s="56">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q30" s="64">
+      <c r="Q30" s="57">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
@@ -5304,12 +5352,14 @@
       <c r="A31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="C31" s="42">
         <f>'Packet Rates'!C43*'Packet Sizes'!C25</f>
         <v>3968</v>
       </c>
-      <c r="D31" s="113">
+      <c r="D31" s="64">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5357,11 +5407,11 @@
         <f t="shared" si="4"/>
         <v>643979</v>
       </c>
-      <c r="P31" s="63">
+      <c r="P31" s="56">
         <f t="shared" si="5"/>
         <v>0.96205964630280538</v>
       </c>
-      <c r="Q31" s="64">
+      <c r="Q31" s="57">
         <f t="shared" si="6"/>
         <v>0.92066734734002742</v>
       </c>
@@ -5370,40 +5420,75 @@
       <c r="A32" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="113">
+      <c r="B32" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="42">
+        <f>'Packet Rates'!C44*'Packet Sizes'!C26</f>
+        <v>3968</v>
+      </c>
+      <c r="D32" s="64">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="63">
+        <v>0.96915422885572144</v>
+      </c>
+      <c r="E32" s="9">
+        <f>'Packet Rates'!E44*'Packet Sizes'!D26</f>
+        <v>11360</v>
+      </c>
+      <c r="F32" s="10">
+        <f>'Packet Rates'!F44*'Packet Sizes'!D26</f>
+        <v>34080</v>
+      </c>
+      <c r="G32" s="10">
+        <f>'Packet Rates'!G44*'Packet Sizes'!E26</f>
+        <v>11040</v>
+      </c>
+      <c r="H32" s="10">
+        <f>'Packet Rates'!H44*'Packet Sizes'!F26</f>
+        <v>6901</v>
+      </c>
+      <c r="I32" s="10">
+        <f>'Packet Rates'!I44*'Packet Sizes'!G26</f>
+        <v>2324</v>
+      </c>
+      <c r="J32" s="10">
+        <f>'Packet Rates'!J44*'Packet Sizes'!H26</f>
+        <v>13280</v>
+      </c>
+      <c r="K32" s="22">
+        <f>'Packet Rates'!K44*'Packet Sizes'!H26</f>
+        <v>39840</v>
+      </c>
+      <c r="L32" s="24">
+        <f t="shared" si="1"/>
+        <v>44905</v>
+      </c>
+      <c r="M32" s="11">
+        <f t="shared" si="7"/>
+        <v>94185</v>
+      </c>
+      <c r="N32" s="24">
+        <f t="shared" si="3"/>
+        <v>314335</v>
+      </c>
+      <c r="O32" s="11">
+        <f t="shared" si="4"/>
+        <v>659295</v>
+      </c>
+      <c r="P32" s="56">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q32" s="64">
+        <v>0.96127664198075946</v>
+      </c>
+      <c r="Q32" s="57">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.91878054837897405</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="34"/>
       <c r="B33" s="35"/>
       <c r="C33" s="42"/>
-      <c r="D33" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D33" s="64"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -5415,23 +5500,14 @@
       <c r="M33" s="14"/>
       <c r="N33" s="25"/>
       <c r="O33" s="26"/>
-      <c r="P33" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q33" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="57"/>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="35"/>
       <c r="C34" s="42"/>
-      <c r="D34" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D34" s="64"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -5443,23 +5519,14 @@
       <c r="M34" s="14"/>
       <c r="N34" s="25"/>
       <c r="O34" s="26"/>
-      <c r="P34" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q34" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="57"/>
     </row>
     <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="42"/>
-      <c r="D35" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D35" s="64"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -5471,23 +5538,14 @@
       <c r="M35" s="14"/>
       <c r="N35" s="25"/>
       <c r="O35" s="26"/>
-      <c r="P35" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q35" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="57"/>
     </row>
     <row r="36" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
       <c r="B36" s="35"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D36" s="64"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -5499,23 +5557,14 @@
       <c r="M36" s="14"/>
       <c r="N36" s="25"/>
       <c r="O36" s="26"/>
-      <c r="P36" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q36" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="57"/>
     </row>
     <row r="37" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
       <c r="B37" s="35"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D37" s="64"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
@@ -5527,23 +5576,14 @@
       <c r="M37" s="14"/>
       <c r="N37" s="25"/>
       <c r="O37" s="26"/>
-      <c r="P37" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q37" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="57"/>
     </row>
     <row r="38" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
       <c r="B38" s="35"/>
       <c r="C38" s="42"/>
-      <c r="D38" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D38" s="64"/>
       <c r="E38" s="12"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
@@ -5555,23 +5595,14 @@
       <c r="M38" s="14"/>
       <c r="N38" s="25"/>
       <c r="O38" s="26"/>
-      <c r="P38" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q38" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="57"/>
     </row>
     <row r="39" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="36"/>
       <c r="B39" s="37"/>
       <c r="C39" s="42"/>
-      <c r="D39" s="113">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="D39" s="64"/>
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -5583,17 +5614,20 @@
       <c r="M39" s="17"/>
       <c r="N39" s="27"/>
       <c r="O39" s="28"/>
-      <c r="P39" s="63">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q39" s="64">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="E15:M15"/>
@@ -5608,21 +5642,12 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="L16:M16"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:D39">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5630,11 +5655,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F39 E18:E20">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="D18:D39">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E20 E21:F39">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5643,10 +5680,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G39">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5655,10 +5692,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H39">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5667,10 +5704,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I39">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5679,10 +5716,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K39">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5691,10 +5728,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:M39">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5703,10 +5740,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:P39">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
@@ -5715,7 +5752,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:P39">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5726,11 +5763,51 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18:Q39">
+  <conditionalFormatting sqref="P18:P32">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="90"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="70"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -5738,11 +5815,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:D39">
+  <conditionalFormatting sqref="Q18:Q32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>

</xml_diff>

<commit_message>
DOC: Update PRooFPS-dd v0.2.8.0 Calculations
</commit_message>
<xml_diff>
--- a/PGE/docpages/PRooFPS-dd-Packet-Rates.xlsx
+++ b/PGE/docpages/PRooFPS-dd-Packet-Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\__PR00F__\___developing___\projects\PGE\PGE\docpages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49CA120-188A-4964-9E4F-AAD31A7C858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F55768-2F80-45F8-A186-71811D254363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3B884228-A0CD-4E16-8D2B-359C9F8D4720}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet Sizes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="91">
   <si>
     <t>v0.1.2</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>Added nMapItemType and nAmmoIncrease to WpnUpdateFromServer.</t>
+  </si>
+  <si>
+    <t>v0.2.8</t>
+  </si>
+  <si>
+    <t>Momentary aim accuracy added to UserUpdateFromServer.</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1077,9 +1083,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1154,15 +1157,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1205,6 +1202,30 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1226,6 +1247,63 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1241,9 +1319,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1268,60 +1343,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1332,30 +1353,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1695,11 +1692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECDFA06-7C74-467D-91F0-6C7F3FAEFF70}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="11" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,30 +1745,30 @@
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
     </row>
     <row r="11" spans="1:18" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="53" t="s">
+      <c r="A11" s="76"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="51" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="19" t="s">
@@ -1798,28 +1795,28 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="111">
+      <c r="C12" s="65">
         <v>268</v>
       </c>
-      <c r="D12" s="112">
+      <c r="D12" s="66">
         <v>268</v>
       </c>
-      <c r="E12" s="113">
+      <c r="E12" s="67">
         <v>268</v>
       </c>
-      <c r="F12" s="113">
+      <c r="F12" s="67">
         <v>268</v>
       </c>
-      <c r="G12" s="113">
+      <c r="G12" s="67">
         <v>268</v>
       </c>
-      <c r="H12" s="114">
+      <c r="H12" s="68">
         <v>268</v>
       </c>
       <c r="I12" s="5"/>
@@ -1830,16 +1827,16 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="41">
         <v>268</v>
       </c>
-      <c r="D13" s="59">
+      <c r="D13" s="56">
         <v>268</v>
       </c>
       <c r="E13" s="10">
@@ -1851,7 +1848,7 @@
       <c r="G13" s="10">
         <v>268</v>
       </c>
-      <c r="H13" s="115">
+      <c r="H13" s="69">
         <v>268</v>
       </c>
       <c r="I13" s="5"/>
@@ -1862,16 +1859,16 @@
       <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>268</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="56">
         <v>268</v>
       </c>
       <c r="E14" s="10">
@@ -1883,7 +1880,7 @@
       <c r="G14" s="10">
         <v>268</v>
       </c>
-      <c r="H14" s="115">
+      <c r="H14" s="69">
         <v>268</v>
       </c>
       <c r="I14" s="5"/>
@@ -1894,16 +1891,16 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="41">
         <v>268</v>
       </c>
-      <c r="D15" s="59">
+      <c r="D15" s="56">
         <v>268</v>
       </c>
       <c r="E15" s="10">
@@ -1915,7 +1912,7 @@
       <c r="G15" s="10">
         <v>268</v>
       </c>
-      <c r="H15" s="115">
+      <c r="H15" s="69">
         <v>268</v>
       </c>
       <c r="I15" s="5"/>
@@ -1926,16 +1923,16 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="41">
         <v>31</v>
       </c>
-      <c r="D16" s="59">
+      <c r="D16" s="56">
         <v>55</v>
       </c>
       <c r="E16" s="10">
@@ -1947,7 +1944,7 @@
       <c r="G16" s="10">
         <v>79</v>
       </c>
-      <c r="H16" s="115">
+      <c r="H16" s="69">
         <v>71</v>
       </c>
       <c r="I16" s="5"/>
@@ -1958,16 +1955,16 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="41">
         <v>31</v>
       </c>
-      <c r="D17" s="59">
+      <c r="D17" s="56">
         <v>55</v>
       </c>
       <c r="E17" s="10">
@@ -1979,7 +1976,7 @@
       <c r="G17" s="10">
         <v>79</v>
       </c>
-      <c r="H17" s="115">
+      <c r="H17" s="69">
         <v>71</v>
       </c>
       <c r="I17" s="5"/>
@@ -1990,16 +1987,16 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="41">
         <v>31</v>
       </c>
-      <c r="D18" s="59">
+      <c r="D18" s="56">
         <v>55</v>
       </c>
       <c r="E18" s="10">
@@ -2011,7 +2008,7 @@
       <c r="G18" s="10">
         <v>79</v>
       </c>
-      <c r="H18" s="115">
+      <c r="H18" s="69">
         <v>71</v>
       </c>
       <c r="I18" s="5"/>
@@ -2022,16 +2019,16 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <v>31</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="56">
         <v>55</v>
       </c>
       <c r="E19" s="10">
@@ -2043,7 +2040,7 @@
       <c r="G19" s="10">
         <v>79</v>
       </c>
-      <c r="H19" s="115">
+      <c r="H19" s="69">
         <v>83</v>
       </c>
       <c r="I19" s="5"/>
@@ -2054,16 +2051,16 @@
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="41">
         <v>31</v>
       </c>
-      <c r="D20" s="59">
+      <c r="D20" s="56">
         <v>55</v>
       </c>
       <c r="E20" s="10">
@@ -2075,7 +2072,7 @@
       <c r="G20" s="10">
         <v>79</v>
       </c>
-      <c r="H20" s="115">
+      <c r="H20" s="69">
         <v>83</v>
       </c>
       <c r="I20" s="5"/>
@@ -2086,16 +2083,16 @@
       <c r="N20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="41">
         <v>31</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="56">
         <v>63</v>
       </c>
       <c r="E21" s="10">
@@ -2107,7 +2104,7 @@
       <c r="G21" s="10">
         <v>79</v>
       </c>
-      <c r="H21" s="115">
+      <c r="H21" s="69">
         <v>83</v>
       </c>
       <c r="I21" s="5"/>
@@ -2118,16 +2115,16 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="41">
         <v>31</v>
       </c>
-      <c r="D22" s="59">
+      <c r="D22" s="56">
         <v>67</v>
       </c>
       <c r="E22" s="10">
@@ -2139,7 +2136,7 @@
       <c r="G22" s="10">
         <v>83</v>
       </c>
-      <c r="H22" s="115">
+      <c r="H22" s="69">
         <v>83</v>
       </c>
       <c r="I22" s="5"/>
@@ -2150,16 +2147,16 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="41">
         <v>31</v>
       </c>
-      <c r="D23" s="59">
+      <c r="D23" s="56">
         <v>67</v>
       </c>
       <c r="E23" s="10">
@@ -2171,7 +2168,7 @@
       <c r="G23" s="10">
         <v>83</v>
       </c>
-      <c r="H23" s="115">
+      <c r="H23" s="69">
         <v>83</v>
       </c>
       <c r="I23" s="5"/>
@@ -2182,16 +2179,16 @@
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="41">
         <v>31</v>
       </c>
-      <c r="D24" s="59">
+      <c r="D24" s="56">
         <v>67</v>
       </c>
       <c r="E24" s="10">
@@ -2203,7 +2200,7 @@
       <c r="G24" s="10">
         <v>83</v>
       </c>
-      <c r="H24" s="115">
+      <c r="H24" s="69">
         <v>83</v>
       </c>
       <c r="I24" s="5"/>
@@ -2214,16 +2211,16 @@
       <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="41">
         <v>31</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="56">
         <v>67</v>
       </c>
       <c r="E25" s="10">
@@ -2235,7 +2232,7 @@
       <c r="G25" s="10">
         <v>83</v>
       </c>
-      <c r="H25" s="115">
+      <c r="H25" s="69">
         <v>83</v>
       </c>
       <c r="I25" s="5"/>
@@ -2246,17 +2243,17 @@
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="109" t="s">
+      <c r="B26" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="41">
         <f>16+15</f>
         <v>31</v>
       </c>
-      <c r="D26" s="59">
+      <c r="D26" s="56">
         <f>56+15</f>
         <v>71</v>
       </c>
@@ -2272,7 +2269,7 @@
         <f>68+15</f>
         <v>83</v>
       </c>
-      <c r="H26" s="115">
+      <c r="H26" s="69">
         <f>68+15</f>
         <v>83</v>
       </c>
@@ -2283,15 +2280,37 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="32"/>
+    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="41">
+        <f>16+15</f>
+        <v>31</v>
+      </c>
+      <c r="D27" s="56">
+        <f>60+15</f>
+        <v>75</v>
+      </c>
+      <c r="E27" s="10">
+        <f>8+15</f>
+        <v>23</v>
+      </c>
+      <c r="F27" s="10">
+        <f>88+15</f>
+        <v>103</v>
+      </c>
+      <c r="G27" s="10">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
+      <c r="H27" s="69">
+        <f>68+15</f>
+        <v>83</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -2300,14 +2319,14 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="109"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="32"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="69"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -2316,14 +2335,14 @@
       <c r="N28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="32"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="69"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -2332,14 +2351,14 @@
       <c r="N29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="109"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="32"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="69"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2348,14 +2367,14 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="32"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="69"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -2364,14 +2383,14 @@
       <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="32"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="69"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -2380,14 +2399,14 @@
       <c r="N32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="32"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="69"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -2396,14 +2415,14 @@
       <c r="N33" s="5"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="47"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="46"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2529,10 +2548,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C73525B-4602-4ED0-8F77-5C69A22A2F34}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A22" sqref="A22"/>
-      <selection pane="topRight" activeCell="E35" sqref="E35"/>
+      <selection pane="topRight" activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,91 +2729,91 @@
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="86" t="s">
+      <c r="A27" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="94" t="s">
+      <c r="C27" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="96"/>
-      <c r="E27" s="97" t="s">
+      <c r="D27" s="87"/>
+      <c r="E27" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="97"/>
-      <c r="K27" s="97"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="97"/>
-      <c r="N27" s="94" t="s">
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="96"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="87"/>
     </row>
     <row r="28" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="74" t="s">
+      <c r="A28" s="78"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="80" t="s">
+      <c r="D28" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77" t="s">
+      <c r="F28" s="91"/>
+      <c r="G28" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="101" t="s">
+      <c r="H28" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="77" t="s">
+      <c r="I28" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="77" t="s">
+      <c r="J28" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="103"/>
-      <c r="L28" s="78" t="s">
+      <c r="K28" s="95"/>
+      <c r="L28" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="79"/>
-      <c r="N28" s="98" t="s">
+      <c r="M28" s="102"/>
+      <c r="N28" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="99"/>
-      <c r="P28" s="92" t="s">
+      <c r="O28" s="90"/>
+      <c r="P28" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="Q28" s="93"/>
+      <c r="Q28" s="84"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="88"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="81"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="104"/>
       <c r="E29" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="100"/>
-      <c r="H29" s="102"/>
-      <c r="I29" s="100"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="92"/>
       <c r="J29" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="38" t="s">
+      <c r="K29" s="37" t="s">
         <v>64</v>
       </c>
       <c r="L29" s="18" t="s">
@@ -2817,25 +2836,25 @@
       </c>
     </row>
     <row r="30" spans="1:23" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="40">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="D30" s="60">
+      <c r="D30" s="57">
         <f>1-(C30/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="85">
+      <c r="E30" s="108">
         <f>$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="F30" s="82"/>
+      <c r="F30" s="105"/>
       <c r="G30" s="7">
         <f>$C$10*$C$13</f>
         <v>480</v>
@@ -2848,20 +2867,20 @@
         <f>$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J30" s="82">
+      <c r="J30" s="105">
         <f>$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K30" s="83"/>
-      <c r="L30" s="23">
-        <f t="shared" ref="L30:L44" si="0">E30+G30+H30+I30+J30</f>
+      <c r="K30" s="106"/>
+      <c r="L30" s="22">
+        <f t="shared" ref="L30:L45" si="0">E30+G30+H30+I30+J30</f>
         <v>4327</v>
       </c>
       <c r="M30" s="8">
         <f>E30+G30+H30+I30+J30</f>
         <v>4327</v>
       </c>
-      <c r="N30" s="23">
+      <c r="N30" s="22">
         <f>7*L30</f>
         <v>30289</v>
       </c>
@@ -2869,11 +2888,11 @@
         <f>7*M30</f>
         <v>30289</v>
       </c>
-      <c r="P30" s="56">
+      <c r="P30" s="53">
         <f>1-(N30/$N$30)</f>
         <v>0</v>
       </c>
-      <c r="Q30" s="57">
+      <c r="Q30" s="54">
         <f>1-(O30/$O$30)</f>
         <v>0</v>
       </c>
@@ -2885,25 +2904,25 @@
       <c r="W30" s="4"/>
     </row>
     <row r="31" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="41">
         <f t="shared" ref="C31:G33" si="1">$C$10*$C$13</f>
         <v>480</v>
       </c>
-      <c r="D31" s="61">
-        <f t="shared" ref="D31:D51" si="2">1-(C31/$C$30)</f>
+      <c r="D31" s="58">
+        <f t="shared" ref="D31:D44" si="2">1-(C31/$C$30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="72">
+      <c r="E31" s="96">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F31" s="73"/>
+      <c r="F31" s="97"/>
       <c r="G31" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2916,12 +2935,12 @@
         <f t="shared" ref="I31:I33" si="4">$C$9*$C$13</f>
         <v>420</v>
       </c>
-      <c r="J31" s="73">
+      <c r="J31" s="97">
         <f t="shared" ref="J31:J32" si="5">$C$11*$C$13</f>
         <v>2880</v>
       </c>
-      <c r="K31" s="84"/>
-      <c r="L31" s="24">
+      <c r="K31" s="107"/>
+      <c r="L31" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
       </c>
@@ -2929,20 +2948,20 @@
         <f>E31+G31+H31+I31+J31</f>
         <v>4327</v>
       </c>
-      <c r="N31" s="24">
-        <f t="shared" ref="N31:N44" si="6">7*L31</f>
+      <c r="N31" s="23">
+        <f t="shared" ref="N31:N45" si="6">7*L31</f>
         <v>30289</v>
       </c>
       <c r="O31" s="11">
-        <f t="shared" ref="O31:O44" si="7">7*M31</f>
+        <f t="shared" ref="O31:O45" si="7">7*M31</f>
         <v>30289</v>
       </c>
-      <c r="P31" s="56">
-        <f t="shared" ref="P31:P51" si="8">1-(N31/$N$30)</f>
+      <c r="P31" s="53">
+        <f t="shared" ref="P31:P45" si="8">1-(N31/$N$30)</f>
         <v>0</v>
       </c>
-      <c r="Q31" s="57">
-        <f t="shared" ref="Q31:Q51" si="9">1-(O31/$O$30)</f>
+      <c r="Q31" s="54">
+        <f t="shared" ref="Q31:Q45" si="9">1-(O31/$O$30)</f>
         <v>0</v>
       </c>
       <c r="R31" s="4"/>
@@ -2953,25 +2972,25 @@
       <c r="W31" s="4"/>
     </row>
     <row r="32" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="41">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E32" s="72">
+      <c r="E32" s="96">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="F32" s="73"/>
+      <c r="F32" s="97"/>
       <c r="G32" s="10">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -2984,12 +3003,12 @@
         <f t="shared" si="4"/>
         <v>420</v>
       </c>
-      <c r="J32" s="73">
+      <c r="J32" s="97">
         <f t="shared" si="5"/>
         <v>2880</v>
       </c>
-      <c r="K32" s="84"/>
-      <c r="L32" s="24">
+      <c r="K32" s="107"/>
+      <c r="L32" s="23">
         <f t="shared" si="0"/>
         <v>4327</v>
       </c>
@@ -2997,7 +3016,7 @@
         <f>E32+G32+H32+I32+J32</f>
         <v>4327</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="23">
         <f t="shared" si="6"/>
         <v>30289</v>
       </c>
@@ -3005,11 +3024,11 @@
         <f t="shared" si="7"/>
         <v>30289</v>
       </c>
-      <c r="P32" s="56">
+      <c r="P32" s="53">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="57">
+      <c r="Q32" s="54">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3021,25 +3040,25 @@
       <c r="W32" s="4"/>
     </row>
     <row r="33" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="41">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D33" s="61">
+      <c r="D33" s="58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E33" s="72">
+      <c r="E33" s="96">
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F33" s="73"/>
+      <c r="F33" s="97"/>
       <c r="G33" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3056,11 +3075,11 @@
         <f>$C$11*$C$15</f>
         <v>960</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="21">
         <f>$C$11*$C$15</f>
         <v>960</v>
       </c>
-      <c r="L33" s="24">
+      <c r="L33" s="23">
         <f t="shared" si="0"/>
         <v>1727</v>
       </c>
@@ -3068,7 +3087,7 @@
         <f>E33+G33+H33+I33+K33</f>
         <v>1727</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="23">
         <f t="shared" si="6"/>
         <v>12089</v>
       </c>
@@ -3076,11 +3095,11 @@
         <f t="shared" si="7"/>
         <v>12089</v>
       </c>
-      <c r="P33" s="56">
+      <c r="P33" s="53">
         <f t="shared" si="8"/>
         <v>0.60087820660966029</v>
       </c>
-      <c r="Q33" s="57">
+      <c r="Q33" s="54">
         <f t="shared" si="9"/>
         <v>0.60087820660966029</v>
       </c>
@@ -3092,25 +3111,25 @@
       <c r="W33" s="4"/>
     </row>
     <row r="34" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="41">
         <f>16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D34" s="61">
+      <c r="D34" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
-      <c r="E34" s="72">
+      <c r="E34" s="96">
         <f t="shared" ref="E34" si="10">$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="F34" s="73"/>
+      <c r="F34" s="97"/>
       <c r="G34" s="10">
         <f>$C$10*$C$15</f>
         <v>160</v>
@@ -3127,11 +3146,11 @@
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="21">
         <f>$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="L34" s="24">
+      <c r="L34" s="23">
         <f t="shared" si="0"/>
         <v>521</v>
       </c>
@@ -3139,7 +3158,7 @@
         <f>E34+G34+H34+I34+K34</f>
         <v>521</v>
       </c>
-      <c r="N34" s="24">
+      <c r="N34" s="23">
         <f t="shared" si="6"/>
         <v>3647</v>
       </c>
@@ -3147,11 +3166,11 @@
         <f t="shared" si="7"/>
         <v>3647</v>
       </c>
-      <c r="P34" s="56">
+      <c r="P34" s="53">
         <f t="shared" si="8"/>
         <v>0.87959325167552582</v>
       </c>
-      <c r="Q34" s="57">
+      <c r="Q34" s="54">
         <f t="shared" si="9"/>
         <v>0.87959325167552582</v>
       </c>
@@ -3163,17 +3182,17 @@
       <c r="W34" s="4"/>
     </row>
     <row r="35" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="42">
-        <f t="shared" ref="C35:C44" si="11">16*$C$10</f>
+      <c r="C35" s="41">
+        <f t="shared" ref="C35:C45" si="11">16*$C$10</f>
         <v>128</v>
       </c>
-      <c r="D35" s="61">
+      <c r="D35" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3182,14 +3201,14 @@
         <v>160</v>
       </c>
       <c r="F35" s="10">
-        <f t="shared" ref="F35:F44" si="12">$C$10*$C$16</f>
+        <f t="shared" ref="F35:F45" si="12">$C$10*$C$16</f>
         <v>480</v>
       </c>
       <c r="G35" s="10">
         <f>$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="21">
         <f>7 + 1*$C$13</f>
         <v>67</v>
       </c>
@@ -3198,22 +3217,22 @@
         <v>14</v>
       </c>
       <c r="J35" s="10">
-        <f t="shared" ref="J35:J44" si="14">$C$10*$C$15</f>
+        <f t="shared" ref="J35:J45" si="14">$C$10*$C$15</f>
         <v>160</v>
       </c>
-      <c r="K35" s="22">
-        <f t="shared" ref="K35:K44" si="15">$C$10*$C$14</f>
+      <c r="K35" s="21">
+        <f t="shared" ref="K35:K45" si="15">$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L35" s="23">
         <f t="shared" si="0"/>
         <v>881</v>
       </c>
       <c r="M35" s="11">
-        <f t="shared" ref="M35:M44" si="16">F35+G35+H35+I35+K35</f>
+        <f t="shared" ref="M35:M45" si="16">F35+G35+H35+I35+K35</f>
         <v>1521</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N35" s="23">
         <f t="shared" si="6"/>
         <v>6167</v>
       </c>
@@ -3221,11 +3240,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P35" s="56">
+      <c r="P35" s="53">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q35" s="57">
+      <c r="Q35" s="54">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3237,22 +3256,22 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="42">
+      <c r="C36" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D36" s="61">
+      <c r="D36" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
       <c r="E36" s="9">
-        <f t="shared" ref="E36:E44" si="17">$C$10*$C$17</f>
+        <f t="shared" ref="E36:E45" si="17">$C$10*$C$17</f>
         <v>160</v>
       </c>
       <c r="F36" s="10">
@@ -3260,11 +3279,11 @@
         <v>480</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" ref="G36:G44" si="18">$C$10*$C$14</f>
+        <f t="shared" ref="G36:G45" si="18">$C$10*$C$14</f>
         <v>480</v>
       </c>
-      <c r="H36" s="22">
-        <f t="shared" ref="H36:H44" si="19">7 + 1*$C$13</f>
+      <c r="H36" s="21">
+        <f t="shared" ref="H36:H45" si="19">7 + 1*$C$13</f>
         <v>67</v>
       </c>
       <c r="I36" s="10">
@@ -3275,11 +3294,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L36" s="24">
+      <c r="L36" s="23">
         <f t="shared" si="0"/>
         <v>881</v>
       </c>
@@ -3287,7 +3306,7 @@
         <f t="shared" si="16"/>
         <v>1521</v>
       </c>
-      <c r="N36" s="24">
+      <c r="N36" s="23">
         <f t="shared" si="6"/>
         <v>6167</v>
       </c>
@@ -3295,11 +3314,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P36" s="56">
+      <c r="P36" s="53">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q36" s="57">
+      <c r="Q36" s="54">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3311,17 +3330,17 @@
       <c r="W36" s="4"/>
     </row>
     <row r="37" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="42">
+      <c r="C37" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D37" s="61">
+      <c r="D37" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3337,7 +3356,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3349,11 +3368,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L37" s="24">
+      <c r="L37" s="23">
         <f t="shared" si="0"/>
         <v>881</v>
       </c>
@@ -3361,7 +3380,7 @@
         <f t="shared" si="16"/>
         <v>1521</v>
       </c>
-      <c r="N37" s="24">
+      <c r="N37" s="23">
         <f t="shared" si="6"/>
         <v>6167</v>
       </c>
@@ -3369,11 +3388,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P37" s="56">
+      <c r="P37" s="53">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q37" s="57">
+      <c r="Q37" s="54">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3385,17 +3404,17 @@
       <c r="W37" s="4"/>
     </row>
     <row r="38" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="42">
+      <c r="C38" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D38" s="61">
+      <c r="D38" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3411,7 +3430,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3423,11 +3442,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K38" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L38" s="24">
+      <c r="L38" s="23">
         <f t="shared" si="0"/>
         <v>881</v>
       </c>
@@ -3435,7 +3454,7 @@
         <f t="shared" si="16"/>
         <v>1521</v>
       </c>
-      <c r="N38" s="24">
+      <c r="N38" s="23">
         <f t="shared" si="6"/>
         <v>6167</v>
       </c>
@@ -3443,11 +3462,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P38" s="56">
+      <c r="P38" s="53">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q38" s="57">
+      <c r="Q38" s="54">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3459,17 +3478,17 @@
       <c r="W38" s="4"/>
     </row>
     <row r="39" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="42">
+      <c r="C39" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D39" s="61">
+      <c r="D39" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3485,7 +3504,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3497,11 +3516,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L39" s="24">
+      <c r="L39" s="23">
         <f t="shared" si="0"/>
         <v>881</v>
       </c>
@@ -3509,7 +3528,7 @@
         <f t="shared" si="16"/>
         <v>1521</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="23">
         <f t="shared" si="6"/>
         <v>6167</v>
       </c>
@@ -3517,11 +3536,11 @@
         <f t="shared" si="7"/>
         <v>10647</v>
       </c>
-      <c r="P39" s="56">
+      <c r="P39" s="53">
         <f t="shared" si="8"/>
         <v>0.79639473076034206</v>
       </c>
-      <c r="Q39" s="57">
+      <c r="Q39" s="54">
         <f t="shared" si="9"/>
         <v>0.64848624913334874</v>
       </c>
@@ -3533,17 +3552,17 @@
       <c r="W39" s="4"/>
     </row>
     <row r="40" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="42">
+      <c r="C40" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D40" s="61">
+      <c r="D40" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3559,7 +3578,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3571,11 +3590,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L40" s="24">
+      <c r="L40" s="23">
         <f t="shared" si="0"/>
         <v>895</v>
       </c>
@@ -3583,7 +3602,7 @@
         <f t="shared" si="16"/>
         <v>1535</v>
       </c>
-      <c r="N40" s="24">
+      <c r="N40" s="23">
         <f t="shared" si="6"/>
         <v>6265</v>
       </c>
@@ -3591,11 +3610,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P40" s="56">
+      <c r="P40" s="53">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q40" s="57">
+      <c r="Q40" s="54">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3607,17 +3626,17 @@
       <c r="W40" s="4"/>
     </row>
     <row r="41" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="42">
+      <c r="C41" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D41" s="61">
+      <c r="D41" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3633,23 +3652,23 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" ref="I41:I44" si="20">$C$9*2 + $C$9*2</f>
+        <f t="shared" ref="I41:I45" si="20">$C$9*2 + $C$9*2</f>
         <v>28</v>
       </c>
       <c r="J41" s="10">
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L41" s="24">
+      <c r="L41" s="23">
         <f t="shared" si="0"/>
         <v>895</v>
       </c>
@@ -3657,7 +3676,7 @@
         <f t="shared" si="16"/>
         <v>1535</v>
       </c>
-      <c r="N41" s="24">
+      <c r="N41" s="23">
         <f t="shared" si="6"/>
         <v>6265</v>
       </c>
@@ -3665,11 +3684,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P41" s="56">
+      <c r="P41" s="53">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q41" s="57">
+      <c r="Q41" s="54">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3681,17 +3700,17 @@
       <c r="W41" s="4"/>
     </row>
     <row r="42" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="42">
+      <c r="C42" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D42" s="61">
+      <c r="D42" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3707,7 +3726,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3719,11 +3738,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K42" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L42" s="24">
+      <c r="L42" s="23">
         <f t="shared" si="0"/>
         <v>895</v>
       </c>
@@ -3731,7 +3750,7 @@
         <f t="shared" si="16"/>
         <v>1535</v>
       </c>
-      <c r="N42" s="24">
+      <c r="N42" s="23">
         <f t="shared" si="6"/>
         <v>6265</v>
       </c>
@@ -3739,11 +3758,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P42" s="56">
+      <c r="P42" s="53">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q42" s="57">
+      <c r="Q42" s="54">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3755,17 +3774,17 @@
       <c r="W42" s="4"/>
     </row>
     <row r="43" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="42">
+      <c r="C43" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D43" s="61">
+      <c r="D43" s="58">
         <f t="shared" si="2"/>
         <v>0.73333333333333339</v>
       </c>
@@ -3781,7 +3800,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H43" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3793,11 +3812,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K43" s="22">
+      <c r="K43" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L43" s="24">
+      <c r="L43" s="23">
         <f t="shared" si="0"/>
         <v>895</v>
       </c>
@@ -3805,7 +3824,7 @@
         <f t="shared" si="16"/>
         <v>1535</v>
       </c>
-      <c r="N43" s="24">
+      <c r="N43" s="23">
         <f t="shared" si="6"/>
         <v>6265</v>
       </c>
@@ -3813,11 +3832,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P43" s="56">
+      <c r="P43" s="53">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q43" s="57">
+      <c r="Q43" s="54">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3829,18 +3848,18 @@
       <c r="W43" s="4"/>
     </row>
     <row r="44" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="41">
         <f t="shared" si="11"/>
         <v>128</v>
       </c>
-      <c r="D44" s="61">
-        <f t="shared" si="2"/>
+      <c r="D44" s="58">
+        <f>1-(C44/$C$30)</f>
         <v>0.73333333333333339</v>
       </c>
       <c r="E44" s="9">
@@ -3855,7 +3874,7 @@
         <f t="shared" si="18"/>
         <v>480</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="21">
         <f t="shared" si="19"/>
         <v>67</v>
       </c>
@@ -3867,11 +3886,11 @@
         <f t="shared" si="14"/>
         <v>160</v>
       </c>
-      <c r="K44" s="22">
+      <c r="K44" s="21">
         <f t="shared" si="15"/>
         <v>480</v>
       </c>
-      <c r="L44" s="24">
+      <c r="L44" s="23">
         <f t="shared" si="0"/>
         <v>895</v>
       </c>
@@ -3879,7 +3898,7 @@
         <f t="shared" si="16"/>
         <v>1535</v>
       </c>
-      <c r="N44" s="24">
+      <c r="N44" s="23">
         <f t="shared" si="6"/>
         <v>6265</v>
       </c>
@@ -3887,11 +3906,11 @@
         <f t="shared" si="7"/>
         <v>10745</v>
       </c>
-      <c r="P44" s="56">
+      <c r="P44" s="53">
         <f t="shared" si="8"/>
         <v>0.79315923272475153</v>
       </c>
-      <c r="Q44" s="57">
+      <c r="Q44" s="54">
         <f t="shared" si="9"/>
         <v>0.64525075109775831</v>
       </c>
@@ -3903,23 +3922,72 @@
       <c r="W44" s="4"/>
     </row>
     <row r="45" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="57"/>
+      <c r="A45" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="41">
+        <f t="shared" si="11"/>
+        <v>128</v>
+      </c>
+      <c r="D45" s="58">
+        <f>1-(C45/$C$30)</f>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="E45" s="9">
+        <f t="shared" si="17"/>
+        <v>160</v>
+      </c>
+      <c r="F45" s="10">
+        <f t="shared" si="12"/>
+        <v>480</v>
+      </c>
+      <c r="G45" s="10">
+        <f t="shared" si="18"/>
+        <v>480</v>
+      </c>
+      <c r="H45" s="21">
+        <f t="shared" si="19"/>
+        <v>67</v>
+      </c>
+      <c r="I45" s="10">
+        <f t="shared" si="20"/>
+        <v>28</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="14"/>
+        <v>160</v>
+      </c>
+      <c r="K45" s="21">
+        <f t="shared" si="15"/>
+        <v>480</v>
+      </c>
+      <c r="L45" s="23">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
+      <c r="M45" s="11">
+        <f t="shared" si="16"/>
+        <v>1535</v>
+      </c>
+      <c r="N45" s="23">
+        <f t="shared" si="6"/>
+        <v>6265</v>
+      </c>
+      <c r="O45" s="11">
+        <f t="shared" si="7"/>
+        <v>10745</v>
+      </c>
+      <c r="P45" s="53">
+        <f t="shared" si="8"/>
+        <v>0.79315923272475153</v>
+      </c>
+      <c r="Q45" s="54">
+        <f t="shared" si="9"/>
+        <v>0.64525075109775831</v>
+      </c>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
@@ -3928,23 +3996,23 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="61"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="58"/>
       <c r="E46" s="12"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="25"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="24"/>
       <c r="M46" s="14"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="26"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="57"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="25"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="54"/>
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
@@ -3953,23 +4021,23 @@
       <c r="W46" s="4"/>
     </row>
     <row r="47" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="61"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="12"/>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="25"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="24"/>
       <c r="M47" s="14"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="26"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="57"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="54"/>
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
@@ -3978,23 +4046,23 @@
       <c r="W47" s="4"/>
     </row>
     <row r="48" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="61"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="58"/>
       <c r="E48" s="12"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="25"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="24"/>
       <c r="M48" s="14"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="26"/>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="57"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="54"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
       <c r="T48" s="4"/>
@@ -4003,23 +4071,23 @@
       <c r="W48" s="4"/>
     </row>
     <row r="49" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="61"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="58"/>
       <c r="E49" s="12"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="25"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="24"/>
       <c r="M49" s="14"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="26"/>
-      <c r="P49" s="56"/>
-      <c r="Q49" s="57"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="54"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
@@ -4028,23 +4096,23 @@
       <c r="W49" s="4"/>
     </row>
     <row r="50" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="61"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="58"/>
       <c r="E50" s="12"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="25"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="24"/>
       <c r="M50" s="14"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="26"/>
-      <c r="P50" s="56"/>
-      <c r="Q50" s="57"/>
+      <c r="N50" s="24"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="54"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
@@ -4053,23 +4121,23 @@
       <c r="W50" s="4"/>
     </row>
     <row r="51" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="61"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="58"/>
       <c r="E51" s="15"/>
       <c r="F51" s="16"/>
       <c r="G51" s="16"/>
       <c r="H51" s="16"/>
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="27"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="26"/>
       <c r="M51" s="17"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="28"/>
-      <c r="P51" s="56"/>
-      <c r="Q51" s="57"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="27"/>
+      <c r="P51" s="53"/>
+      <c r="Q51" s="54"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
@@ -4080,7 +4148,7 @@
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="62"/>
+      <c r="D52" s="59"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -4092,8 +4160,8 @@
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
-      <c r="P52" s="58"/>
-      <c r="Q52" s="58"/>
+      <c r="P52" s="55"/>
+      <c r="Q52" s="55"/>
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
@@ -4160,17 +4228,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="C28:C29"/>
@@ -4183,6 +4240,17 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="C30:D51">
     <cfRule type="colorScale" priority="17">
@@ -4280,7 +4348,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P30:Q44">
+  <conditionalFormatting sqref="N30:O45">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="30"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P30:Q45">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4292,18 +4372,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30:O44">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percent" val="30"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4312,9 +4380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A631036-56BD-4CE5-917C-895C0C771D72}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C27" sqref="C27"/>
+      <selection pane="topRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4382,91 +4450,91 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="97" t="s">
+      <c r="D15" s="87"/>
+      <c r="E15" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="94" t="s">
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="96"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="87"/>
     </row>
     <row r="16" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="74" t="s">
+      <c r="A16" s="78"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="103" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77" t="s">
+      <c r="F16" s="91"/>
+      <c r="G16" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="101" t="s">
+      <c r="H16" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="77" t="s">
+      <c r="I16" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="77" t="s">
+      <c r="J16" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="103"/>
-      <c r="L16" s="78" t="s">
+      <c r="K16" s="95"/>
+      <c r="L16" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="79"/>
-      <c r="N16" s="98" t="s">
+      <c r="M16" s="102"/>
+      <c r="N16" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="99"/>
-      <c r="P16" s="92" t="s">
+      <c r="O16" s="90"/>
+      <c r="P16" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="93"/>
+      <c r="Q16" s="84"/>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="81"/>
+      <c r="A17" s="79"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="104"/>
       <c r="E17" s="18" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="100"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="100"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="92"/>
       <c r="J17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="38" t="s">
+      <c r="K17" s="37" t="s">
         <v>64</v>
       </c>
       <c r="L17" s="18" t="s">
@@ -4489,25 +4557,25 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="40">
         <f>'Packet Rates'!C30*'Packet Sizes'!C12</f>
         <v>128640</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="60">
         <f>1-(C18/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="104">
+      <c r="E18" s="109">
         <f>'Packet Rates'!E30*'Packet Sizes'!D12</f>
         <v>128640</v>
       </c>
-      <c r="F18" s="105"/>
+      <c r="F18" s="110"/>
       <c r="G18" s="7">
         <f>'Packet Rates'!G30*'Packet Sizes'!E12</f>
         <v>128640</v>
@@ -4520,12 +4588,12 @@
         <f>'Packet Rates'!I30*'Packet Sizes'!G12</f>
         <v>112560</v>
       </c>
-      <c r="J18" s="82">
+      <c r="J18" s="105">
         <f>'Packet Rates'!J30*'Packet Sizes'!H12</f>
         <v>771840</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="23">
+      <c r="K18" s="106"/>
+      <c r="L18" s="22">
         <f>E18+G18+H18+I18+J18</f>
         <v>1159636</v>
       </c>
@@ -4533,7 +4601,7 @@
         <f>E18+G18+H18+I18+J18</f>
         <v>1159636</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="22">
         <f>L18*7</f>
         <v>8117452</v>
       </c>
@@ -4541,35 +4609,35 @@
         <f>M18*7</f>
         <v>8117452</v>
       </c>
-      <c r="P18" s="56">
+      <c r="P18" s="53">
         <f>1-(N18/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="54">
         <f>1-(O18/$O$18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <f>'Packet Rates'!C31*'Packet Sizes'!C13</f>
         <v>128640</v>
       </c>
-      <c r="D19" s="64">
-        <f t="shared" ref="D19:D39" si="0">1-(C19/$C$18)</f>
+      <c r="D19" s="61">
+        <f t="shared" ref="D19:D33" si="0">1-(C19/$C$18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E19" s="111">
         <f>'Packet Rates'!E31*'Packet Sizes'!D13</f>
         <v>128640</v>
       </c>
-      <c r="F19" s="107"/>
+      <c r="F19" s="112"/>
       <c r="G19" s="10">
         <f>'Packet Rates'!G31*'Packet Sizes'!E13</f>
         <v>128640</v>
@@ -4582,56 +4650,56 @@
         <f>'Packet Rates'!I31*'Packet Sizes'!G13</f>
         <v>112560</v>
       </c>
-      <c r="J19" s="73">
+      <c r="J19" s="97">
         <f>'Packet Rates'!J31*'Packet Sizes'!H13</f>
         <v>771840</v>
       </c>
-      <c r="K19" s="84"/>
-      <c r="L19" s="24">
-        <f t="shared" ref="L19:L32" si="1">E19+G19+H19+I19+J19</f>
+      <c r="K19" s="107"/>
+      <c r="L19" s="23">
+        <f t="shared" ref="L19:L33" si="1">E19+G19+H19+I19+J19</f>
         <v>1159636</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" ref="M19:M20" si="2">E19+G19+H19+I19+J19</f>
         <v>1159636</v>
       </c>
-      <c r="N19" s="24">
-        <f t="shared" ref="N19:N32" si="3">L19*7</f>
+      <c r="N19" s="23">
+        <f t="shared" ref="N19:N33" si="3">L19*7</f>
         <v>8117452</v>
       </c>
       <c r="O19" s="11">
-        <f t="shared" ref="O19:O32" si="4">M19*7</f>
+        <f t="shared" ref="O19:O33" si="4">M19*7</f>
         <v>8117452</v>
       </c>
-      <c r="P19" s="56">
-        <f t="shared" ref="P19:P39" si="5">1-(N19/$N$18)</f>
+      <c r="P19" s="53">
+        <f t="shared" ref="P19:P33" si="5">1-(N19/$N$18)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="57">
-        <f t="shared" ref="Q19:Q39" si="6">1-(O19/$O$18)</f>
+      <c r="Q19" s="54">
+        <f t="shared" ref="Q19:Q33" si="6">1-(O19/$O$18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="41">
         <f>'Packet Rates'!C32*'Packet Sizes'!C14</f>
         <v>128640</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="106">
+      <c r="E20" s="111">
         <f>'Packet Rates'!E32*'Packet Sizes'!D14</f>
         <v>128640</v>
       </c>
-      <c r="F20" s="107"/>
+      <c r="F20" s="112"/>
       <c r="G20" s="10">
         <f>'Packet Rates'!G32*'Packet Sizes'!E14</f>
         <v>128640</v>
@@ -4644,12 +4712,12 @@
         <f>'Packet Rates'!I32*'Packet Sizes'!G14</f>
         <v>112560</v>
       </c>
-      <c r="J20" s="73">
+      <c r="J20" s="97">
         <f>'Packet Rates'!J32*'Packet Sizes'!H14</f>
         <v>771840</v>
       </c>
-      <c r="K20" s="84"/>
-      <c r="L20" s="24">
+      <c r="K20" s="107"/>
+      <c r="L20" s="23">
         <f t="shared" si="1"/>
         <v>1159636</v>
       </c>
@@ -4657,7 +4725,7 @@
         <f t="shared" si="2"/>
         <v>1159636</v>
       </c>
-      <c r="N20" s="24">
+      <c r="N20" s="23">
         <f t="shared" si="3"/>
         <v>8117452</v>
       </c>
@@ -4665,35 +4733,35 @@
         <f t="shared" si="4"/>
         <v>8117452</v>
       </c>
-      <c r="P20" s="56">
+      <c r="P20" s="53">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="57">
+      <c r="Q20" s="54">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="41">
         <f>'Packet Rates'!C33*'Packet Sizes'!C15</f>
         <v>128640</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D21" s="61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="72">
+      <c r="E21" s="96">
         <f>'Packet Rates'!E33*'Packet Sizes'!D15</f>
         <v>42880</v>
       </c>
-      <c r="F21" s="73"/>
+      <c r="F21" s="97"/>
       <c r="G21" s="10">
         <f>'Packet Rates'!G33*'Packet Sizes'!E15</f>
         <v>42880</v>
@@ -4710,11 +4778,11 @@
         <f>'Packet Rates'!J33*'Packet Sizes'!H15</f>
         <v>257280</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="21">
         <f>'Packet Rates'!K33*'Packet Sizes'!H15</f>
         <v>257280</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="23">
         <f t="shared" si="1"/>
         <v>462836</v>
       </c>
@@ -4722,7 +4790,7 @@
         <f>E21+G21+H21+I21+K21</f>
         <v>462836</v>
       </c>
-      <c r="N21" s="24">
+      <c r="N21" s="23">
         <f t="shared" si="3"/>
         <v>3239852</v>
       </c>
@@ -4730,35 +4798,35 @@
         <f t="shared" si="4"/>
         <v>3239852</v>
       </c>
-      <c r="P21" s="56">
+      <c r="P21" s="53">
         <f t="shared" si="5"/>
         <v>0.60087820660966029</v>
       </c>
-      <c r="Q21" s="57">
+      <c r="Q21" s="54">
         <f t="shared" si="6"/>
         <v>0.60087820660966029</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="41">
         <f>'Packet Rates'!C34*'Packet Sizes'!C16</f>
         <v>3968</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
-      <c r="E22" s="72">
+      <c r="E22" s="96">
         <f>'Packet Rates'!E34*'Packet Sizes'!D16</f>
         <v>8800</v>
       </c>
-      <c r="F22" s="73"/>
+      <c r="F22" s="97"/>
       <c r="G22" s="10">
         <f>'Packet Rates'!G34*'Packet Sizes'!E16</f>
         <v>3680</v>
@@ -4775,11 +4843,11 @@
         <f>'Packet Rates'!J34*'Packet Sizes'!H16</f>
         <v>11360</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="21">
         <f>'Packet Rates'!K34*'Packet Sizes'!H16</f>
         <v>11360</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="23">
         <f t="shared" si="1"/>
         <v>27403</v>
       </c>
@@ -4787,7 +4855,7 @@
         <f>E22+G22+H22+I22+K22</f>
         <v>27403</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="23">
         <f t="shared" si="3"/>
         <v>191821</v>
       </c>
@@ -4795,27 +4863,27 @@
         <f t="shared" si="4"/>
         <v>191821</v>
       </c>
-      <c r="P22" s="56">
+      <c r="P22" s="53">
         <f t="shared" si="5"/>
         <v>0.97636930899006236</v>
       </c>
-      <c r="Q22" s="57">
+      <c r="Q22" s="54">
         <f t="shared" si="6"/>
         <v>0.97636930899006236</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="41">
         <f>'Packet Rates'!C35*'Packet Sizes'!C17</f>
         <v>3968</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4843,11 +4911,11 @@
         <f>'Packet Rates'!J35*'Packet Sizes'!H17</f>
         <v>11360</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="21">
         <f>'Packet Rates'!K35*'Packet Sizes'!H17</f>
         <v>34080</v>
       </c>
-      <c r="L23" s="24">
+      <c r="L23" s="23">
         <f t="shared" si="1"/>
         <v>38403</v>
       </c>
@@ -4855,7 +4923,7 @@
         <f>F23+G23+H23+I23+K23</f>
         <v>78723</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23" s="23">
         <f t="shared" si="3"/>
         <v>268821</v>
       </c>
@@ -4863,27 +4931,27 @@
         <f t="shared" si="4"/>
         <v>551061</v>
       </c>
-      <c r="P23" s="56">
+      <c r="P23" s="53">
         <f t="shared" si="5"/>
         <v>0.96688357381109247</v>
       </c>
-      <c r="Q23" s="57">
+      <c r="Q23" s="54">
         <f t="shared" si="6"/>
         <v>0.93211404268235898</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="41">
         <f>'Packet Rates'!C36*'Packet Sizes'!C18</f>
         <v>3968</v>
       </c>
-      <c r="D24" s="64">
+      <c r="D24" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4911,19 +4979,19 @@
         <f>'Packet Rates'!J36*'Packet Sizes'!H18</f>
         <v>11360</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="21">
         <f>'Packet Rates'!K36*'Packet Sizes'!H18</f>
         <v>34080</v>
       </c>
-      <c r="L24" s="24">
+      <c r="L24" s="23">
         <f t="shared" si="1"/>
         <v>38403</v>
       </c>
       <c r="M24" s="11">
-        <f t="shared" ref="M24:M32" si="7">F24+G24+H24+I24+K24</f>
+        <f t="shared" ref="M24:M33" si="7">F24+G24+H24+I24+K24</f>
         <v>78723</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="23">
         <f t="shared" si="3"/>
         <v>268821</v>
       </c>
@@ -4931,27 +4999,27 @@
         <f t="shared" si="4"/>
         <v>551061</v>
       </c>
-      <c r="P24" s="56">
+      <c r="P24" s="53">
         <f t="shared" si="5"/>
         <v>0.96688357381109247</v>
       </c>
-      <c r="Q24" s="57">
+      <c r="Q24" s="54">
         <f t="shared" si="6"/>
         <v>0.93211404268235898</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="41">
         <f>'Packet Rates'!C37*'Packet Sizes'!C19</f>
         <v>3968</v>
       </c>
-      <c r="D25" s="64">
+      <c r="D25" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -4979,11 +5047,11 @@
         <f>'Packet Rates'!J37*'Packet Sizes'!H19</f>
         <v>13280</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="21">
         <f>'Packet Rates'!K37*'Packet Sizes'!H19</f>
         <v>39840</v>
       </c>
-      <c r="L25" s="24">
+      <c r="L25" s="23">
         <f t="shared" si="1"/>
         <v>40323</v>
       </c>
@@ -4991,7 +5059,7 @@
         <f t="shared" si="7"/>
         <v>84483</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25" s="23">
         <f t="shared" si="3"/>
         <v>282261</v>
       </c>
@@ -4999,27 +5067,27 @@
         <f t="shared" si="4"/>
         <v>591381</v>
       </c>
-      <c r="P25" s="56">
+      <c r="P25" s="53">
         <f t="shared" si="5"/>
         <v>0.96522788185258135</v>
       </c>
-      <c r="Q25" s="57">
+      <c r="Q25" s="54">
         <f t="shared" si="6"/>
         <v>0.92714696680682562</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="41">
         <f>'Packet Rates'!C38*'Packet Sizes'!C20</f>
         <v>3968</v>
       </c>
-      <c r="D26" s="64">
+      <c r="D26" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5047,11 +5115,11 @@
         <f>'Packet Rates'!J38*'Packet Sizes'!H20</f>
         <v>13280</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="21">
         <f>'Packet Rates'!K38*'Packet Sizes'!H20</f>
         <v>39840</v>
       </c>
-      <c r="L26" s="24">
+      <c r="L26" s="23">
         <f t="shared" si="1"/>
         <v>40323</v>
       </c>
@@ -5059,7 +5127,7 @@
         <f t="shared" si="7"/>
         <v>84483</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26" s="23">
         <f t="shared" si="3"/>
         <v>282261</v>
       </c>
@@ -5067,27 +5135,27 @@
         <f t="shared" si="4"/>
         <v>591381</v>
       </c>
-      <c r="P26" s="56">
+      <c r="P26" s="53">
         <f t="shared" si="5"/>
         <v>0.96522788185258135</v>
       </c>
-      <c r="Q26" s="57">
+      <c r="Q26" s="54">
         <f t="shared" si="6"/>
         <v>0.92714696680682562</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="41">
         <f>'Packet Rates'!C39*'Packet Sizes'!C21</f>
         <v>3968</v>
       </c>
-      <c r="D27" s="64">
+      <c r="D27" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5115,11 +5183,11 @@
         <f>'Packet Rates'!J39*'Packet Sizes'!H21</f>
         <v>13280</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="21">
         <f>'Packet Rates'!K39*'Packet Sizes'!H21</f>
         <v>39840</v>
       </c>
-      <c r="L27" s="24">
+      <c r="L27" s="23">
         <f t="shared" si="1"/>
         <v>41603</v>
       </c>
@@ -5127,7 +5195,7 @@
         <f t="shared" si="7"/>
         <v>88323</v>
       </c>
-      <c r="N27" s="24">
+      <c r="N27" s="23">
         <f t="shared" si="3"/>
         <v>291221</v>
       </c>
@@ -5135,27 +5203,27 @@
         <f t="shared" si="4"/>
         <v>618261</v>
       </c>
-      <c r="P27" s="56">
+      <c r="P27" s="53">
         <f t="shared" si="5"/>
         <v>0.9641240872135739</v>
       </c>
-      <c r="Q27" s="57">
+      <c r="Q27" s="54">
         <f t="shared" si="6"/>
         <v>0.92383558288980339</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="42">
+      <c r="C28" s="41">
         <f>'Packet Rates'!C40*'Packet Sizes'!C22</f>
         <v>3968</v>
       </c>
-      <c r="D28" s="64">
+      <c r="D28" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5183,11 +5251,11 @@
         <f>'Packet Rates'!J40*'Packet Sizes'!H22</f>
         <v>13280</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="21">
         <f>'Packet Rates'!K40*'Packet Sizes'!H22</f>
         <v>39840</v>
       </c>
-      <c r="L28" s="24">
+      <c r="L28" s="23">
         <f t="shared" si="1"/>
         <v>43461</v>
       </c>
@@ -5195,7 +5263,7 @@
         <f t="shared" si="7"/>
         <v>91461</v>
       </c>
-      <c r="N28" s="24">
+      <c r="N28" s="23">
         <f t="shared" si="3"/>
         <v>304227</v>
       </c>
@@ -5203,27 +5271,27 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P28" s="56">
+      <c r="P28" s="53">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q28" s="57">
+      <c r="Q28" s="54">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="42">
+      <c r="C29" s="41">
         <f>'Packet Rates'!C41*'Packet Sizes'!C23</f>
         <v>3968</v>
       </c>
-      <c r="D29" s="64">
+      <c r="D29" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5251,11 +5319,11 @@
         <f>'Packet Rates'!J41*'Packet Sizes'!H23</f>
         <v>13280</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="21">
         <f>'Packet Rates'!K41*'Packet Sizes'!H23</f>
         <v>39840</v>
       </c>
-      <c r="L29" s="24">
+      <c r="L29" s="23">
         <f t="shared" si="1"/>
         <v>43461</v>
       </c>
@@ -5263,7 +5331,7 @@
         <f t="shared" si="7"/>
         <v>91461</v>
       </c>
-      <c r="N29" s="24">
+      <c r="N29" s="23">
         <f t="shared" si="3"/>
         <v>304227</v>
       </c>
@@ -5271,27 +5339,27 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P29" s="56">
+      <c r="P29" s="53">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q29" s="57">
+      <c r="Q29" s="54">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="41">
         <f>'Packet Rates'!C42*'Packet Sizes'!C24</f>
         <v>3968</v>
       </c>
-      <c r="D30" s="64">
+      <c r="D30" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5319,11 +5387,11 @@
         <f>'Packet Rates'!J42*'Packet Sizes'!H24</f>
         <v>13280</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="21">
         <f>'Packet Rates'!K42*'Packet Sizes'!H24</f>
         <v>39840</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="23">
         <f t="shared" si="1"/>
         <v>43461</v>
       </c>
@@ -5331,7 +5399,7 @@
         <f t="shared" si="7"/>
         <v>91461</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="23">
         <f t="shared" si="3"/>
         <v>304227</v>
       </c>
@@ -5339,27 +5407,27 @@
         <f t="shared" si="4"/>
         <v>640227</v>
       </c>
-      <c r="P30" s="56">
+      <c r="P30" s="53">
         <f t="shared" si="5"/>
         <v>0.96252186030788967</v>
       </c>
-      <c r="Q30" s="57">
+      <c r="Q30" s="54">
         <f t="shared" si="6"/>
         <v>0.9211295613451117</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="41">
         <f>'Packet Rates'!C43*'Packet Sizes'!C25</f>
         <v>3968</v>
       </c>
-      <c r="D31" s="64">
+      <c r="D31" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5387,11 +5455,11 @@
         <f>'Packet Rates'!J43*'Packet Sizes'!H25</f>
         <v>13280</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="21">
         <f>'Packet Rates'!K43*'Packet Sizes'!H25</f>
         <v>39840</v>
       </c>
-      <c r="L31" s="24">
+      <c r="L31" s="23">
         <f t="shared" si="1"/>
         <v>43997</v>
       </c>
@@ -5399,7 +5467,7 @@
         <f t="shared" si="7"/>
         <v>91997</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="23">
         <f t="shared" si="3"/>
         <v>307979</v>
       </c>
@@ -5407,27 +5475,27 @@
         <f t="shared" si="4"/>
         <v>643979</v>
       </c>
-      <c r="P31" s="56">
+      <c r="P31" s="53">
         <f t="shared" si="5"/>
         <v>0.96205964630280538</v>
       </c>
-      <c r="Q31" s="57">
+      <c r="Q31" s="54">
         <f t="shared" si="6"/>
         <v>0.92066734734002742</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="41">
         <f>'Packet Rates'!C44*'Packet Sizes'!C26</f>
         <v>3968</v>
       </c>
-      <c r="D32" s="64">
+      <c r="D32" s="61">
         <f t="shared" si="0"/>
         <v>0.96915422885572144</v>
       </c>
@@ -5455,11 +5523,11 @@
         <f>'Packet Rates'!J44*'Packet Sizes'!H26</f>
         <v>13280</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="21">
         <f>'Packet Rates'!K44*'Packet Sizes'!H26</f>
         <v>39840</v>
       </c>
-      <c r="L32" s="24">
+      <c r="L32" s="23">
         <f t="shared" si="1"/>
         <v>44905</v>
       </c>
@@ -5467,7 +5535,7 @@
         <f t="shared" si="7"/>
         <v>94185</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="23">
         <f t="shared" si="3"/>
         <v>314335</v>
       </c>
@@ -5475,159 +5543,199 @@
         <f t="shared" si="4"/>
         <v>659295</v>
       </c>
-      <c r="P32" s="56">
+      <c r="P32" s="53">
         <f t="shared" si="5"/>
         <v>0.96127664198075946</v>
       </c>
-      <c r="Q32" s="57">
+      <c r="Q32" s="54">
         <f t="shared" si="6"/>
         <v>0.91878054837897405</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="57"/>
+      <c r="A33" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="41">
+        <f>'Packet Rates'!C45*'Packet Sizes'!C27</f>
+        <v>3968</v>
+      </c>
+      <c r="D33" s="61">
+        <f t="shared" si="0"/>
+        <v>0.96915422885572144</v>
+      </c>
+      <c r="E33" s="9">
+        <f>'Packet Rates'!E45*'Packet Sizes'!D27</f>
+        <v>12000</v>
+      </c>
+      <c r="F33" s="10">
+        <f>'Packet Rates'!F45*'Packet Sizes'!D27</f>
+        <v>36000</v>
+      </c>
+      <c r="G33" s="10">
+        <f>'Packet Rates'!G45*'Packet Sizes'!E27</f>
+        <v>11040</v>
+      </c>
+      <c r="H33" s="10">
+        <f>'Packet Rates'!H45*'Packet Sizes'!F27</f>
+        <v>6901</v>
+      </c>
+      <c r="I33" s="10">
+        <f>'Packet Rates'!I45*'Packet Sizes'!G27</f>
+        <v>2324</v>
+      </c>
+      <c r="J33" s="10">
+        <f>'Packet Rates'!J45*'Packet Sizes'!H27</f>
+        <v>13280</v>
+      </c>
+      <c r="K33" s="21">
+        <f>'Packet Rates'!K45*'Packet Sizes'!H27</f>
+        <v>39840</v>
+      </c>
+      <c r="L33" s="23">
+        <f t="shared" si="1"/>
+        <v>45545</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="7"/>
+        <v>96105</v>
+      </c>
+      <c r="N33" s="23">
+        <f t="shared" si="3"/>
+        <v>318815</v>
+      </c>
+      <c r="O33" s="11">
+        <f t="shared" si="4"/>
+        <v>672735</v>
+      </c>
+      <c r="P33" s="53">
+        <f t="shared" si="5"/>
+        <v>0.96072474466125579</v>
+      </c>
+      <c r="Q33" s="54">
+        <f t="shared" si="6"/>
+        <v>0.91712485642046293</v>
+      </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="64"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="25"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="24"/>
       <c r="M34" s="14"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="57"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="54"/>
     </row>
     <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="64"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="61"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="25"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="24"/>
       <c r="M35" s="14"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="57"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="54"/>
     </row>
     <row r="36" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="64"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="61"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="25"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="24"/>
       <c r="M36" s="14"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="57"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="54"/>
     </row>
     <row r="37" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="64"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="61"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="25"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="24"/>
       <c r="M37" s="14"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="57"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="54"/>
     </row>
     <row r="38" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="64"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="61"/>
       <c r="E38" s="12"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="25"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="24"/>
       <c r="M38" s="14"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="57"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="54"/>
     </row>
     <row r="39" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="64"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="61"/>
       <c r="E39" s="15"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="27"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="26"/>
       <c r="M39" s="17"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="28"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="57"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="E15:M15"/>
@@ -5642,6 +5750,15 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="C18:D39">
     <cfRule type="colorScale" priority="17">
@@ -5751,33 +5868,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P39">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="P18:P33">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percent" val="70"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P18:P32">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="90"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="10"/>
+        <cfvo type="percent" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -5794,20 +5899,32 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percent" val="50"/>
+        <cfvo type="percentile" val="10"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percent" val="70"/>
+        <cfvo type="percentile" val="90"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18:P39">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -5815,7 +5932,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q18:Q32">
+  <conditionalFormatting sqref="Q18:Q33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>